<commit_message>
MVC UPDATE STS FRESSHH
</commit_message>
<xml_diff>
--- a/temp_doc/PESERTA UJIAN MOODLE XII SAS 2024.xlsx
+++ b/temp_doc/PESERTA UJIAN MOODLE XII SAS 2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/XAMPP/xamppfiles/htdocs/cbt2.0admin/temp_doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B3082CA-82AB-0747-A501-E7744C5562B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC111F33-73C7-3949-BECD-19D7A38DCD76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2315,14 +2315,14 @@
     <t>XII PM</t>
   </si>
   <si>
-    <t>SASTH46@</t>
+    <t>SASTH46</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2462,6 +2462,12 @@
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="33">
@@ -2805,10 +2811,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -3167,7 +3172,7 @@
   <dimension ref="A1:G1042"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="B2" sqref="B2:B247"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3209,7 +3214,7 @@
       <c r="A2" s="1" t="s">
         <v>259</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" t="s">
         <v>760</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -3226,14 +3231,14 @@
       </c>
       <c r="G2" t="str">
         <f t="shared" ref="G2:G65" si="0">CONCATENATE(A2,",",B2,",",C2,",",D2,",",E2,",",F2)</f>
-        <v>K0103009800018,SASTH46@,AGUNG RAMADHAN,(XII TJKT 1),K0103009800018@gmail.com,XII TJKT 1</v>
+        <v>K0103009800018,SASTH46,AGUNG RAMADHAN,(XII TJKT 1),K0103009800018@gmail.com,XII TJKT 1</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" t="s">
         <v>760</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -3250,14 +3255,14 @@
       </c>
       <c r="G3" t="str">
         <f t="shared" si="0"/>
-        <v>K0103009800027,SASTH46@,AHMAD AGUS TAWAKAL,(XII TJKT 1),K0103009800027@gmail.com,XII TJKT 1</v>
+        <v>K0103009800027,SASTH46,AHMAD AGUS TAWAKAL,(XII TJKT 1),K0103009800027@gmail.com,XII TJKT 1</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" t="s">
         <v>760</v>
       </c>
       <c r="C4" s="1" t="s">
@@ -3274,14 +3279,14 @@
       </c>
       <c r="G4" t="str">
         <f t="shared" si="0"/>
-        <v>K0103009800036,SASTH46@,ALFIAN FEBRIYANTO,(XII TJKT 1),K0103009800036@gmail.com,XII TJKT 1</v>
+        <v>K0103009800036,SASTH46,ALFIAN FEBRIYANTO,(XII TJKT 1),K0103009800036@gmail.com,XII TJKT 1</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" t="s">
         <v>760</v>
       </c>
       <c r="C5" s="1" t="s">
@@ -3298,14 +3303,14 @@
       </c>
       <c r="G5" t="str">
         <f t="shared" si="0"/>
-        <v>K0103009800045,SASTH46@,ALFIAN NUR ILHAM,(XII TJKT 1),K0103009800045@gmail.com,XII TJKT 1</v>
+        <v>K0103009800045,SASTH46,ALFIAN NUR ILHAM,(XII TJKT 1),K0103009800045@gmail.com,XII TJKT 1</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" t="s">
         <v>760</v>
       </c>
       <c r="C6" s="1" t="s">
@@ -3322,14 +3327,14 @@
       </c>
       <c r="G6" t="str">
         <f t="shared" si="0"/>
-        <v>K0103009800054,SASTH46@,ALPIN RAMADAN SETIAWAN,(XII TJKT 1),K0103009800054@gmail.com,XII TJKT 1</v>
+        <v>K0103009800054,SASTH46,ALPIN RAMADAN SETIAWAN,(XII TJKT 1),K0103009800054@gmail.com,XII TJKT 1</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" t="s">
         <v>760</v>
       </c>
       <c r="C7" s="1" t="s">
@@ -3346,14 +3351,14 @@
       </c>
       <c r="G7" t="str">
         <f t="shared" si="0"/>
-        <v>K0103009800063,SASTH46@,DENTA FITRI NOVIANI,(XII TJKT 1),K0103009800063@gmail.com,XII TJKT 1</v>
+        <v>K0103009800063,SASTH46,DENTA FITRI NOVIANI,(XII TJKT 1),K0103009800063@gmail.com,XII TJKT 1</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" t="s">
         <v>760</v>
       </c>
       <c r="C8" s="1" t="s">
@@ -3370,14 +3375,14 @@
       </c>
       <c r="G8" t="str">
         <f t="shared" si="0"/>
-        <v>K0103009800072,SASTH46@,EGI KURNIA,(XII TJKT 1),K0103009800072@gmail.com,XII TJKT 1</v>
+        <v>K0103009800072,SASTH46,EGI KURNIA,(XII TJKT 1),K0103009800072@gmail.com,XII TJKT 1</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>266</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" t="s">
         <v>760</v>
       </c>
       <c r="C9" s="1" t="s">
@@ -3394,14 +3399,14 @@
       </c>
       <c r="G9" t="str">
         <f t="shared" si="0"/>
-        <v>K0103009800089,SASTH46@,EGNER CONSTANTIN,(XII TJKT 1),K0103009800089@gmail.com,XII TJKT 1</v>
+        <v>K0103009800089,SASTH46,EGNER CONSTANTIN,(XII TJKT 1),K0103009800089@gmail.com,XII TJKT 1</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" t="s">
         <v>760</v>
       </c>
       <c r="C10" s="1" t="s">
@@ -3418,14 +3423,14 @@
       </c>
       <c r="G10" t="str">
         <f t="shared" si="0"/>
-        <v>K0103009800098,SASTH46@,ERICH JALEMBA JUNIARTA,(XII TJKT 1),K0103009800098@gmail.com,XII TJKT 1</v>
+        <v>K0103009800098,SASTH46,ERICH JALEMBA JUNIARTA,(XII TJKT 1),K0103009800098@gmail.com,XII TJKT 1</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" t="s">
         <v>760</v>
       </c>
       <c r="C11" s="1" t="s">
@@ -3442,14 +3447,14 @@
       </c>
       <c r="G11" t="str">
         <f t="shared" si="0"/>
-        <v>K0103009800107,SASTH46@,FADLY ERLANGGA,(XII TJKT 1),K0103009800107@gmail.com,XII TJKT 1</v>
+        <v>K0103009800107,SASTH46,FADLY ERLANGGA,(XII TJKT 1),K0103009800107@gmail.com,XII TJKT 1</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>269</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" t="s">
         <v>760</v>
       </c>
       <c r="C12" s="1" t="s">
@@ -3466,14 +3471,14 @@
       </c>
       <c r="G12" t="str">
         <f t="shared" si="0"/>
-        <v>K0103009800116,SASTH46@,FATHYA AULIA,(XII TJKT 1),K0103009800116@gmail.com,XII TJKT 1</v>
+        <v>K0103009800116,SASTH46,FATHYA AULIA,(XII TJKT 1),K0103009800116@gmail.com,XII TJKT 1</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>270</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" t="s">
         <v>760</v>
       </c>
       <c r="C13" s="1" t="s">
@@ -3490,14 +3495,14 @@
       </c>
       <c r="G13" t="str">
         <f t="shared" si="0"/>
-        <v>K0103009800125,SASTH46@,FIKHAR HADISAPUTRA,(XII TJKT 1),K0103009800125@gmail.com,XII TJKT 1</v>
+        <v>K0103009800125,SASTH46,FIKHAR HADISAPUTRA,(XII TJKT 1),K0103009800125@gmail.com,XII TJKT 1</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>271</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" t="s">
         <v>760</v>
       </c>
       <c r="C14" s="1" t="s">
@@ -3514,14 +3519,14 @@
       </c>
       <c r="G14" t="str">
         <f t="shared" si="0"/>
-        <v>K0103009800134,SASTH46@,FRANS LEONARDO HADIWINATA,(XII TJKT 1),K0103009800134@gmail.com,XII TJKT 1</v>
+        <v>K0103009800134,SASTH46,FRANS LEONARDO HADIWINATA,(XII TJKT 1),K0103009800134@gmail.com,XII TJKT 1</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" t="s">
         <v>760</v>
       </c>
       <c r="C15" s="1" t="s">
@@ -3538,14 +3543,14 @@
       </c>
       <c r="G15" t="str">
         <f t="shared" si="0"/>
-        <v>K0103009800143,SASTH46@,GILANG MAULANA AKBAR,(XII TJKT 1),K0103009800143@gmail.com,XII TJKT 1</v>
+        <v>K0103009800143,SASTH46,GILANG MAULANA AKBAR,(XII TJKT 1),K0103009800143@gmail.com,XII TJKT 1</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>273</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" t="s">
         <v>760</v>
       </c>
       <c r="C16" s="1" t="s">
@@ -3562,14 +3567,14 @@
       </c>
       <c r="G16" t="str">
         <f t="shared" si="0"/>
-        <v>K0103009800152,SASTH46@,HAFIDZ SYAHPUTRO,(XII TJKT 1),K0103009800152@gmail.com,XII TJKT 1</v>
+        <v>K0103009800152,SASTH46,HAFIDZ SYAHPUTRO,(XII TJKT 1),K0103009800152@gmail.com,XII TJKT 1</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" t="s">
         <v>760</v>
       </c>
       <c r="C17" s="1" t="s">
@@ -3586,14 +3591,14 @@
       </c>
       <c r="G17" t="str">
         <f t="shared" si="0"/>
-        <v>K0103009800169,SASTH46@,KELVIN OKTA RAMADHAN,(XII TJKT 1),K0103009800169@gmail.com,XII TJKT 1</v>
+        <v>K0103009800169,SASTH46,KELVIN OKTA RAMADHAN,(XII TJKT 1),K0103009800169@gmail.com,XII TJKT 1</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>275</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" t="s">
         <v>760</v>
       </c>
       <c r="C18" s="1" t="s">
@@ -3610,14 +3615,14 @@
       </c>
       <c r="G18" t="str">
         <f t="shared" si="0"/>
-        <v>K0103009800178,SASTH46@,MAULANA IKSAN,(XII TJKT 1),K0103009800178@gmail.com,XII TJKT 1</v>
+        <v>K0103009800178,SASTH46,MAULANA IKSAN,(XII TJKT 1),K0103009800178@gmail.com,XII TJKT 1</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" t="s">
         <v>760</v>
       </c>
       <c r="C19" s="1" t="s">
@@ -3634,14 +3639,14 @@
       </c>
       <c r="G19" t="str">
         <f t="shared" si="0"/>
-        <v>K0103009800187,SASTH46@,MOHAMAD RIZKI,(XII TJKT 1),K0103009800187@gmail.com,XII TJKT 1</v>
+        <v>K0103009800187,SASTH46,MOHAMAD RIZKI,(XII TJKT 1),K0103009800187@gmail.com,XII TJKT 1</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>277</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" t="s">
         <v>760</v>
       </c>
       <c r="C20" s="1" t="s">
@@ -3658,14 +3663,14 @@
       </c>
       <c r="G20" t="str">
         <f t="shared" si="0"/>
-        <v>K0103009800196,SASTH46@,MUHAMAD SUBASTIAN,(XII TJKT 1),K0103009800196@gmail.com,XII TJKT 1</v>
+        <v>K0103009800196,SASTH46,MUHAMAD SUBASTIAN,(XII TJKT 1),K0103009800196@gmail.com,XII TJKT 1</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>278</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" t="s">
         <v>760</v>
       </c>
       <c r="C21" s="1" t="s">
@@ -3682,14 +3687,14 @@
       </c>
       <c r="G21" t="str">
         <f t="shared" si="0"/>
-        <v>K0103009800205,SASTH46@,MUHAMMAD ANGGI SAPUTRA,(XII TJKT 1),K0103009800205@gmail.com,XII TJKT 1</v>
+        <v>K0103009800205,SASTH46,MUHAMMAD ANGGI SAPUTRA,(XII TJKT 1),K0103009800205@gmail.com,XII TJKT 1</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>279</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B22" t="s">
         <v>760</v>
       </c>
       <c r="C22" s="1" t="s">
@@ -3706,14 +3711,14 @@
       </c>
       <c r="G22" t="str">
         <f t="shared" si="0"/>
-        <v>K0103009800214,SASTH46@,MUHAMMAD NUR ARIFIN,(XII TJKT 1),K0103009800214@gmail.com,XII TJKT 1</v>
+        <v>K0103009800214,SASTH46,MUHAMMAD NUR ARIFIN,(XII TJKT 1),K0103009800214@gmail.com,XII TJKT 1</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B23" t="s">
         <v>760</v>
       </c>
       <c r="C23" s="1" t="s">
@@ -3730,14 +3735,14 @@
       </c>
       <c r="G23" t="str">
         <f t="shared" si="0"/>
-        <v>K0103009800223,SASTH46@,MUHAMMAD RIZKY AL AKBAR,(XII TJKT 1),K0103009800223@gmail.com,XII TJKT 1</v>
+        <v>K0103009800223,SASTH46,MUHAMMAD RIZKY AL AKBAR,(XII TJKT 1),K0103009800223@gmail.com,XII TJKT 1</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>281</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B24" t="s">
         <v>760</v>
       </c>
       <c r="C24" s="1" t="s">
@@ -3754,14 +3759,14 @@
       </c>
       <c r="G24" t="str">
         <f t="shared" si="0"/>
-        <v>K0103009800232,SASTH46@,NOVAL RAMADAN,(XII TJKT 1),K0103009800232@gmail.com,XII TJKT 1</v>
+        <v>K0103009800232,SASTH46,NOVAL RAMADAN,(XII TJKT 1),K0103009800232@gmail.com,XII TJKT 1</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>282</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B25" t="s">
         <v>760</v>
       </c>
       <c r="C25" s="1" t="s">
@@ -3778,14 +3783,14 @@
       </c>
       <c r="G25" t="str">
         <f t="shared" si="0"/>
-        <v>K0103009800249,SASTH46@,NOVEL SYAHPUTRA HALIM,(XII TJKT 1),K0103009800249@gmail.com,XII TJKT 1</v>
+        <v>K0103009800249,SASTH46,NOVEL SYAHPUTRA HALIM,(XII TJKT 1),K0103009800249@gmail.com,XII TJKT 1</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>283</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B26" t="s">
         <v>760</v>
       </c>
       <c r="C26" s="1" t="s">
@@ -3802,14 +3807,14 @@
       </c>
       <c r="G26" t="str">
         <f t="shared" si="0"/>
-        <v>K0103009800258,SASTH46@,PANJI RAHMADI,(XII TJKT 1),K0103009800258@gmail.com,XII TJKT 1</v>
+        <v>K0103009800258,SASTH46,PANJI RAHMADI,(XII TJKT 1),K0103009800258@gmail.com,XII TJKT 1</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>284</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B27" t="s">
         <v>760</v>
       </c>
       <c r="C27" s="1" t="s">
@@ -3826,14 +3831,14 @@
       </c>
       <c r="G27" t="str">
         <f t="shared" si="0"/>
-        <v>K0103009800267,SASTH46@,RADIS SETIAWAN,(XII TJKT 1),K0103009800267@gmail.com,XII TJKT 1</v>
+        <v>K0103009800267,SASTH46,RADIS SETIAWAN,(XII TJKT 1),K0103009800267@gmail.com,XII TJKT 1</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B28" t="s">
         <v>760</v>
       </c>
       <c r="C28" s="1" t="s">
@@ -3850,14 +3855,14 @@
       </c>
       <c r="G28" t="str">
         <f t="shared" si="0"/>
-        <v>K0103009800276,SASTH46@,RAFA MAULANA ARDIANSYAH,(XII TJKT 1),K0103009800276@gmail.com,XII TJKT 1</v>
+        <v>K0103009800276,SASTH46,RAFA MAULANA ARDIANSYAH,(XII TJKT 1),K0103009800276@gmail.com,XII TJKT 1</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>286</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B29" t="s">
         <v>760</v>
       </c>
       <c r="C29" s="1" t="s">
@@ -3874,14 +3879,14 @@
       </c>
       <c r="G29" t="str">
         <f t="shared" si="0"/>
-        <v>K0103009800285,SASTH46@,RAFLI AGUNG PRAYOGA,(XII TJKT 1),K0103009800285@gmail.com,XII TJKT 1</v>
+        <v>K0103009800285,SASTH46,RAFLI AGUNG PRAYOGA,(XII TJKT 1),K0103009800285@gmail.com,XII TJKT 1</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>287</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="B30" t="s">
         <v>760</v>
       </c>
       <c r="C30" s="1" t="s">
@@ -3898,14 +3903,14 @@
       </c>
       <c r="G30" t="str">
         <f t="shared" si="0"/>
-        <v>K0103009800294,SASTH46@,SIGIT NURCAHYONO,(XII TJKT 1),K0103009800294@gmail.com,XII TJKT 1</v>
+        <v>K0103009800294,SASTH46,SIGIT NURCAHYONO,(XII TJKT 1),K0103009800294@gmail.com,XII TJKT 1</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>288</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="B31" t="s">
         <v>760</v>
       </c>
       <c r="C31" s="1" t="s">
@@ -3922,14 +3927,14 @@
       </c>
       <c r="G31" t="str">
         <f t="shared" si="0"/>
-        <v>K0103009800303,SASTH46@,TYO RIYADI SYAPUTRA,(XII TJKT 1),K0103009800303@gmail.com,XII TJKT 1</v>
+        <v>K0103009800303,SASTH46,TYO RIYADI SYAPUTRA,(XII TJKT 1),K0103009800303@gmail.com,XII TJKT 1</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>289</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="B32" t="s">
         <v>760</v>
       </c>
       <c r="C32" s="1" t="s">
@@ -3946,14 +3951,14 @@
       </c>
       <c r="G32" t="str">
         <f t="shared" si="0"/>
-        <v>K0103009800312,SASTH46@,YULIO LUKAS ADRIANO HUTAGAOL,(XII TJKT 1),K0103009800312@gmail.com,XII TJKT 1</v>
+        <v>K0103009800312,SASTH46,YULIO LUKAS ADRIANO HUTAGAOL,(XII TJKT 1),K0103009800312@gmail.com,XII TJKT 1</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>290</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="B33" t="s">
         <v>760</v>
       </c>
       <c r="C33" s="1" t="s">
@@ -3970,14 +3975,14 @@
       </c>
       <c r="G33" t="str">
         <f t="shared" si="0"/>
-        <v>K0103009800329,SASTH46@,ADE IRSAD ABIDIN,(XII TJKT 2),K0103009800329@gmail.com,XII TJKT 2</v>
+        <v>K0103009800329,SASTH46,ADE IRSAD ABIDIN,(XII TJKT 2),K0103009800329@gmail.com,XII TJKT 2</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>291</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="B34" t="s">
         <v>760</v>
       </c>
       <c r="C34" s="1" t="s">
@@ -3994,14 +3999,14 @@
       </c>
       <c r="G34" t="str">
         <f t="shared" si="0"/>
-        <v>K0103009800338,SASTH46@,AFRIZAL ARDIANSYAH,(XII TJKT 2),K0103009800338@gmail.com,XII TJKT 2</v>
+        <v>K0103009800338,SASTH46,AFRIZAL ARDIANSYAH,(XII TJKT 2),K0103009800338@gmail.com,XII TJKT 2</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>292</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="B35" t="s">
         <v>760</v>
       </c>
       <c r="C35" s="1" t="s">
@@ -4018,14 +4023,14 @@
       </c>
       <c r="G35" t="str">
         <f t="shared" si="0"/>
-        <v>K0103009800347,SASTH46@,AHMAD NUR MUDZAKI,(XII TJKT 2),K0103009800347@gmail.com,XII TJKT 2</v>
+        <v>K0103009800347,SASTH46,AHMAD NUR MUDZAKI,(XII TJKT 2),K0103009800347@gmail.com,XII TJKT 2</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>293</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="B36" t="s">
         <v>760</v>
       </c>
       <c r="C36" s="1" t="s">
@@ -4042,14 +4047,14 @@
       </c>
       <c r="G36" t="str">
         <f t="shared" si="0"/>
-        <v>K0103009800356,SASTH46@,ALBASRAH MOHAMAD SALEH RAGO,(XII TJKT 2),K0103009800356@gmail.com,XII TJKT 2</v>
+        <v>K0103009800356,SASTH46,ALBASRAH MOHAMAD SALEH RAGO,(XII TJKT 2),K0103009800356@gmail.com,XII TJKT 2</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>294</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="B37" t="s">
         <v>760</v>
       </c>
       <c r="C37" s="1" t="s">
@@ -4066,14 +4071,14 @@
       </c>
       <c r="G37" t="str">
         <f t="shared" si="0"/>
-        <v>K0103009800365,SASTH46@,ALDI AWALUDIN,(XII TJKT 2),K0103009800365@gmail.com,XII TJKT 2</v>
+        <v>K0103009800365,SASTH46,ALDI AWALUDIN,(XII TJKT 2),K0103009800365@gmail.com,XII TJKT 2</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>295</v>
       </c>
-      <c r="B38" s="2" t="s">
+      <c r="B38" t="s">
         <v>760</v>
       </c>
       <c r="C38" s="1" t="s">
@@ -4090,14 +4095,14 @@
       </c>
       <c r="G38" t="str">
         <f t="shared" si="0"/>
-        <v>K0103009800374,SASTH46@,ANDIKA,(XII TJKT 2),K0103009800374@gmail.com,XII TJKT 2</v>
+        <v>K0103009800374,SASTH46,ANDIKA,(XII TJKT 2),K0103009800374@gmail.com,XII TJKT 2</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>296</v>
       </c>
-      <c r="B39" s="2" t="s">
+      <c r="B39" t="s">
         <v>760</v>
       </c>
       <c r="C39" s="1" t="s">
@@ -4114,14 +4119,14 @@
       </c>
       <c r="G39" t="str">
         <f t="shared" si="0"/>
-        <v>K0103009800383,SASTH46@,ARDESTA KURNIAWAN,(XII TJKT 2),K0103009800383@gmail.com,XII TJKT 2</v>
+        <v>K0103009800383,SASTH46,ARDESTA KURNIAWAN,(XII TJKT 2),K0103009800383@gmail.com,XII TJKT 2</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>297</v>
       </c>
-      <c r="B40" s="2" t="s">
+      <c r="B40" t="s">
         <v>760</v>
       </c>
       <c r="C40" s="1" t="s">
@@ -4138,14 +4143,14 @@
       </c>
       <c r="G40" t="str">
         <f t="shared" si="0"/>
-        <v>K0103009800392,SASTH46@,ARDI DANU ANGGARA,(XII TJKT 2),K0103009800392@gmail.com,XII TJKT 2</v>
+        <v>K0103009800392,SASTH46,ARDI DANU ANGGARA,(XII TJKT 2),K0103009800392@gmail.com,XII TJKT 2</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>298</v>
       </c>
-      <c r="B41" s="2" t="s">
+      <c r="B41" t="s">
         <v>760</v>
       </c>
       <c r="C41" s="1" t="s">
@@ -4162,14 +4167,14 @@
       </c>
       <c r="G41" t="str">
         <f t="shared" si="0"/>
-        <v>K0103009800409,SASTH46@,ARIEL ILHAMI,(XII TJKT 2),K0103009800409@gmail.com,XII TJKT 2</v>
+        <v>K0103009800409,SASTH46,ARIEL ILHAMI,(XII TJKT 2),K0103009800409@gmail.com,XII TJKT 2</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>299</v>
       </c>
-      <c r="B42" s="2" t="s">
+      <c r="B42" t="s">
         <v>760</v>
       </c>
       <c r="C42" s="1" t="s">
@@ -4186,14 +4191,14 @@
       </c>
       <c r="G42" t="str">
         <f t="shared" si="0"/>
-        <v>K0103009800418,SASTH46@,BAYU SAPUTRA,(XII TJKT 2),K0103009800418@gmail.com,XII TJKT 2</v>
+        <v>K0103009800418,SASTH46,BAYU SAPUTRA,(XII TJKT 2),K0103009800418@gmail.com,XII TJKT 2</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>300</v>
       </c>
-      <c r="B43" s="2" t="s">
+      <c r="B43" t="s">
         <v>760</v>
       </c>
       <c r="C43" s="1" t="s">
@@ -4210,14 +4215,14 @@
       </c>
       <c r="G43" t="str">
         <f t="shared" si="0"/>
-        <v>K0103009800427,SASTH46@,DAMARUDIN,(XII TJKT 2),K0103009800427@gmail.com,XII TJKT 2</v>
+        <v>K0103009800427,SASTH46,DAMARUDIN,(XII TJKT 2),K0103009800427@gmail.com,XII TJKT 2</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>301</v>
       </c>
-      <c r="B44" s="2" t="s">
+      <c r="B44" t="s">
         <v>760</v>
       </c>
       <c r="C44" s="1" t="s">
@@ -4234,14 +4239,14 @@
       </c>
       <c r="G44" t="str">
         <f t="shared" si="0"/>
-        <v>K0103009800436,SASTH46@,DEDI MARDIYANSAH,(XII TJKT 2),K0103009800436@gmail.com,XII TJKT 2</v>
+        <v>K0103009800436,SASTH46,DEDI MARDIYANSAH,(XII TJKT 2),K0103009800436@gmail.com,XII TJKT 2</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>302</v>
       </c>
-      <c r="B45" s="2" t="s">
+      <c r="B45" t="s">
         <v>760</v>
       </c>
       <c r="C45" s="1" t="s">
@@ -4258,14 +4263,14 @@
       </c>
       <c r="G45" t="str">
         <f t="shared" si="0"/>
-        <v>K0103009800445,SASTH46@,DEVFRAN ADITYA SUHERNO PUTRA,(XII TJKT 2),K0103009800445@gmail.com,XII TJKT 2</v>
+        <v>K0103009800445,SASTH46,DEVFRAN ADITYA SUHERNO PUTRA,(XII TJKT 2),K0103009800445@gmail.com,XII TJKT 2</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>303</v>
       </c>
-      <c r="B46" s="2" t="s">
+      <c r="B46" t="s">
         <v>760</v>
       </c>
       <c r="C46" s="1" t="s">
@@ -4282,14 +4287,14 @@
       </c>
       <c r="G46" t="str">
         <f t="shared" si="0"/>
-        <v>K0103009800454,SASTH46@,DHIMAS KURNIAWAN BASORI,(XII TJKT 2),K0103009800454@gmail.com,XII TJKT 2</v>
+        <v>K0103009800454,SASTH46,DHIMAS KURNIAWAN BASORI,(XII TJKT 2),K0103009800454@gmail.com,XII TJKT 2</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>304</v>
       </c>
-      <c r="B47" s="2" t="s">
+      <c r="B47" t="s">
         <v>760</v>
       </c>
       <c r="C47" s="1" t="s">
@@ -4306,14 +4311,14 @@
       </c>
       <c r="G47" t="str">
         <f t="shared" si="0"/>
-        <v>K0103009800463,SASTH46@,DIKI RAMADAN,(XII TJKT 2),K0103009800463@gmail.com,XII TJKT 2</v>
+        <v>K0103009800463,SASTH46,DIKI RAMADAN,(XII TJKT 2),K0103009800463@gmail.com,XII TJKT 2</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>305</v>
       </c>
-      <c r="B48" s="2" t="s">
+      <c r="B48" t="s">
         <v>760</v>
       </c>
       <c r="C48" s="1" t="s">
@@ -4330,14 +4335,14 @@
       </c>
       <c r="G48" t="str">
         <f t="shared" si="0"/>
-        <v>K0103009800472,SASTH46@,FAJAR NUGRAHA,(XII TJKT 2),K0103009800472@gmail.com,XII TJKT 2</v>
+        <v>K0103009800472,SASTH46,FAJAR NUGRAHA,(XII TJKT 2),K0103009800472@gmail.com,XII TJKT 2</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="B49" s="2" t="s">
+      <c r="B49" t="s">
         <v>760</v>
       </c>
       <c r="C49" s="1" t="s">
@@ -4354,14 +4359,14 @@
       </c>
       <c r="G49" t="str">
         <f t="shared" si="0"/>
-        <v>K0103009800489,SASTH46@,FIKRI FAHREZA,(XII TJKT 2),K0103009800489@gmail.com,XII TJKT 2</v>
+        <v>K0103009800489,SASTH46,FIKRI FAHREZA,(XII TJKT 2),K0103009800489@gmail.com,XII TJKT 2</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>307</v>
       </c>
-      <c r="B50" s="2" t="s">
+      <c r="B50" t="s">
         <v>760</v>
       </c>
       <c r="C50" s="1" t="s">
@@ -4378,14 +4383,14 @@
       </c>
       <c r="G50" t="str">
         <f t="shared" si="0"/>
-        <v>K0103009800498,SASTH46@,FIRMANSYAH,(XII TJKT 2),K0103009800498@gmail.com,XII TJKT 2</v>
+        <v>K0103009800498,SASTH46,FIRMANSYAH,(XII TJKT 2),K0103009800498@gmail.com,XII TJKT 2</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>308</v>
       </c>
-      <c r="B51" s="2" t="s">
+      <c r="B51" t="s">
         <v>760</v>
       </c>
       <c r="C51" s="1" t="s">
@@ -4402,14 +4407,14 @@
       </c>
       <c r="G51" t="str">
         <f t="shared" si="0"/>
-        <v>K0103009800507,SASTH46@,HABIB SUF'YAN FADILLAH,(XII TJKT 2),K0103009800507@gmail.com,XII TJKT 2</v>
+        <v>K0103009800507,SASTH46,HABIB SUF'YAN FADILLAH,(XII TJKT 2),K0103009800507@gmail.com,XII TJKT 2</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>309</v>
       </c>
-      <c r="B52" s="2" t="s">
+      <c r="B52" t="s">
         <v>760</v>
       </c>
       <c r="C52" s="1" t="s">
@@ -4426,14 +4431,14 @@
       </c>
       <c r="G52" t="str">
         <f t="shared" si="0"/>
-        <v>K0103009800516,SASTH46@,HAIKAL FIKRI NURWANTO,(XII TJKT 2),K0103009800516@gmail.com,XII TJKT 2</v>
+        <v>K0103009800516,SASTH46,HAIKAL FIKRI NURWANTO,(XII TJKT 2),K0103009800516@gmail.com,XII TJKT 2</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>310</v>
       </c>
-      <c r="B53" s="2" t="s">
+      <c r="B53" t="s">
         <v>760</v>
       </c>
       <c r="C53" s="1" t="s">
@@ -4450,14 +4455,14 @@
       </c>
       <c r="G53" t="str">
         <f t="shared" si="0"/>
-        <v>K0103009800525,SASTH46@,I PT.GALIHANDRA REVA ULUM DINATA,(XII TJKT 2),K0103009800525@gmail.com,XII TJKT 2</v>
+        <v>K0103009800525,SASTH46,I PT.GALIHANDRA REVA ULUM DINATA,(XII TJKT 2),K0103009800525@gmail.com,XII TJKT 2</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>311</v>
       </c>
-      <c r="B54" s="2" t="s">
+      <c r="B54" t="s">
         <v>760</v>
       </c>
       <c r="C54" s="1" t="s">
@@ -4474,14 +4479,14 @@
       </c>
       <c r="G54" t="str">
         <f t="shared" si="0"/>
-        <v>K0103009800534,SASTH46@,ILHAM RAHMATTULLOH,(XII TJKT 2),K0103009800534@gmail.com,XII TJKT 2</v>
+        <v>K0103009800534,SASTH46,ILHAM RAHMATTULLOH,(XII TJKT 2),K0103009800534@gmail.com,XII TJKT 2</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>312</v>
       </c>
-      <c r="B55" s="2" t="s">
+      <c r="B55" t="s">
         <v>760</v>
       </c>
       <c r="C55" s="1" t="s">
@@ -4498,14 +4503,14 @@
       </c>
       <c r="G55" t="str">
         <f t="shared" si="0"/>
-        <v>K0103009800543,SASTH46@,INDAH FAAKHIRA SEBASTIAN,(XII TJKT 2),K0103009800543@gmail.com,XII TJKT 2</v>
+        <v>K0103009800543,SASTH46,INDAH FAAKHIRA SEBASTIAN,(XII TJKT 2),K0103009800543@gmail.com,XII TJKT 2</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>313</v>
       </c>
-      <c r="B56" s="2" t="s">
+      <c r="B56" t="s">
         <v>760</v>
       </c>
       <c r="C56" s="1" t="s">
@@ -4522,14 +4527,14 @@
       </c>
       <c r="G56" t="str">
         <f t="shared" si="0"/>
-        <v>K0103009800552,SASTH46@,KEFIN HIDAYAT,(XII TJKT 2),K0103009800552@gmail.com,XII TJKT 2</v>
+        <v>K0103009800552,SASTH46,KEFIN HIDAYAT,(XII TJKT 2),K0103009800552@gmail.com,XII TJKT 2</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>314</v>
       </c>
-      <c r="B57" s="2" t="s">
+      <c r="B57" t="s">
         <v>760</v>
       </c>
       <c r="C57" s="1" t="s">
@@ -4546,14 +4551,14 @@
       </c>
       <c r="G57" t="str">
         <f t="shared" si="0"/>
-        <v>K0103009800569,SASTH46@,MUHAMAD ARDIANSYAH,(XII TJKT 2),K0103009800569@gmail.com,XII TJKT 2</v>
+        <v>K0103009800569,SASTH46,MUHAMAD ARDIANSYAH,(XII TJKT 2),K0103009800569@gmail.com,XII TJKT 2</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>315</v>
       </c>
-      <c r="B58" s="2" t="s">
+      <c r="B58" t="s">
         <v>760</v>
       </c>
       <c r="C58" s="1" t="s">
@@ -4570,14 +4575,14 @@
       </c>
       <c r="G58" t="str">
         <f t="shared" si="0"/>
-        <v>K0103009800578,SASTH46@,MUHAMMAD MAULANA RAMDHANI,(XII TJKT 2),K0103009800578@gmail.com,XII TJKT 2</v>
+        <v>K0103009800578,SASTH46,MUHAMMAD MAULANA RAMDHANI,(XII TJKT 2),K0103009800578@gmail.com,XII TJKT 2</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>316</v>
       </c>
-      <c r="B59" s="2" t="s">
+      <c r="B59" t="s">
         <v>760</v>
       </c>
       <c r="C59" s="1" t="s">
@@ -4594,14 +4599,14 @@
       </c>
       <c r="G59" t="str">
         <f t="shared" si="0"/>
-        <v>K0103009800587,SASTH46@,MUHAMMAD NANDA FIRMANSYAH,(XII TJKT 2),K0103009800587@gmail.com,XII TJKT 2</v>
+        <v>K0103009800587,SASTH46,MUHAMMAD NANDA FIRMANSYAH,(XII TJKT 2),K0103009800587@gmail.com,XII TJKT 2</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>317</v>
       </c>
-      <c r="B60" s="2" t="s">
+      <c r="B60" t="s">
         <v>760</v>
       </c>
       <c r="C60" s="1" t="s">
@@ -4618,14 +4623,14 @@
       </c>
       <c r="G60" t="str">
         <f t="shared" si="0"/>
-        <v>K0103009800596,SASTH46@,MUHAMMAD RIFKI RABBANI,(XII TJKT 2),K0103009800596@gmail.com,XII TJKT 2</v>
+        <v>K0103009800596,SASTH46,MUHAMMAD RIFKI RABBANI,(XII TJKT 2),K0103009800596@gmail.com,XII TJKT 2</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>318</v>
       </c>
-      <c r="B61" s="2" t="s">
+      <c r="B61" t="s">
         <v>760</v>
       </c>
       <c r="C61" s="1" t="s">
@@ -4642,14 +4647,14 @@
       </c>
       <c r="G61" t="str">
         <f t="shared" si="0"/>
-        <v>K0103009800605,SASTH46@,NADIA NURLITA,(XII TJKT 2),K0103009800605@gmail.com,XII TJKT 2</v>
+        <v>K0103009800605,SASTH46,NADIA NURLITA,(XII TJKT 2),K0103009800605@gmail.com,XII TJKT 2</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>319</v>
       </c>
-      <c r="B62" s="2" t="s">
+      <c r="B62" t="s">
         <v>760</v>
       </c>
       <c r="C62" s="1" t="s">
@@ -4666,14 +4671,14 @@
       </c>
       <c r="G62" t="str">
         <f t="shared" si="0"/>
-        <v>K0103009800614,SASTH46@,PINDY AUGY SEPTIANU PUTRA,(XII TJKT 2),K0103009800614@gmail.com,XII TJKT 2</v>
+        <v>K0103009800614,SASTH46,PINDY AUGY SEPTIANU PUTRA,(XII TJKT 2),K0103009800614@gmail.com,XII TJKT 2</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>320</v>
       </c>
-      <c r="B63" s="2" t="s">
+      <c r="B63" t="s">
         <v>760</v>
       </c>
       <c r="C63" s="1" t="s">
@@ -4690,14 +4695,14 @@
       </c>
       <c r="G63" t="str">
         <f t="shared" si="0"/>
-        <v>K0103009800623,SASTH46@,RIFQI AZHAR SAPUTRA,(XII TJKT 2),K0103009800623@gmail.com,XII TJKT 2</v>
+        <v>K0103009800623,SASTH46,RIFQI AZHAR SAPUTRA,(XII TJKT 2),K0103009800623@gmail.com,XII TJKT 2</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
         <v>321</v>
       </c>
-      <c r="B64" s="2" t="s">
+      <c r="B64" t="s">
         <v>760</v>
       </c>
       <c r="C64" s="1" t="s">
@@ -4714,14 +4719,14 @@
       </c>
       <c r="G64" t="str">
         <f t="shared" si="0"/>
-        <v>K0103009800632,SASTH46@,RIZKY BAGASKORO,(XII TJKT 2),K0103009800632@gmail.com,XII TJKT 2</v>
+        <v>K0103009800632,SASTH46,RIZKY BAGASKORO,(XII TJKT 2),K0103009800632@gmail.com,XII TJKT 2</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
         <v>322</v>
       </c>
-      <c r="B65" s="2" t="s">
+      <c r="B65" t="s">
         <v>760</v>
       </c>
       <c r="C65" s="1" t="s">
@@ -4738,14 +4743,14 @@
       </c>
       <c r="G65" t="str">
         <f t="shared" si="0"/>
-        <v>K0103009800649,SASTH46@,ROFIQY MIRYAL AL MURTADHA,(XII TJKT 2),K0103009800649@gmail.com,XII TJKT 2</v>
+        <v>K0103009800649,SASTH46,ROFIQY MIRYAL AL MURTADHA,(XII TJKT 2),K0103009800649@gmail.com,XII TJKT 2</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
         <v>323</v>
       </c>
-      <c r="B66" s="2" t="s">
+      <c r="B66" t="s">
         <v>760</v>
       </c>
       <c r="C66" s="1" t="s">
@@ -4762,14 +4767,14 @@
       </c>
       <c r="G66" t="str">
         <f t="shared" ref="G66:G129" si="1">CONCATENATE(A66,",",B66,",",C66,",",D66,",",E66,",",F66)</f>
-        <v>K0103009800658,SASTH46@,SATRIAWAN TRIE SAPUTRA,(XII TJKT 2),K0103009800658@gmail.com,XII TJKT 2</v>
+        <v>K0103009800658,SASTH46,SATRIAWAN TRIE SAPUTRA,(XII TJKT 2),K0103009800658@gmail.com,XII TJKT 2</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
         <v>324</v>
       </c>
-      <c r="B67" s="2" t="s">
+      <c r="B67" t="s">
         <v>760</v>
       </c>
       <c r="C67" s="1" t="s">
@@ -4786,14 +4791,14 @@
       </c>
       <c r="G67" t="str">
         <f t="shared" si="1"/>
-        <v>K0103009800667,SASTH46@,SUTINAH,(XII TJKT 2),K0103009800667@gmail.com,XII TJKT 2</v>
+        <v>K0103009800667,SASTH46,SUTINAH,(XII TJKT 2),K0103009800667@gmail.com,XII TJKT 2</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
         <v>325</v>
       </c>
-      <c r="B68" s="2" t="s">
+      <c r="B68" t="s">
         <v>760</v>
       </c>
       <c r="C68" s="1" t="s">
@@ -4810,14 +4815,14 @@
       </c>
       <c r="G68" t="str">
         <f t="shared" si="1"/>
-        <v>K0103009800676,SASTH46@,AHMAD SAPUTRA,(XII TJKT 3),K0103009800676@gmail.com,XII TJKT 3</v>
+        <v>K0103009800676,SASTH46,AHMAD SAPUTRA,(XII TJKT 3),K0103009800676@gmail.com,XII TJKT 3</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
         <v>326</v>
       </c>
-      <c r="B69" s="2" t="s">
+      <c r="B69" t="s">
         <v>760</v>
       </c>
       <c r="C69" s="1" t="s">
@@ -4834,14 +4839,14 @@
       </c>
       <c r="G69" t="str">
         <f t="shared" si="1"/>
-        <v>K0103009800685,SASTH46@,ANDYKA PUTRA PRASETYA,(XII TJKT 3),K0103009800685@gmail.com,XII TJKT 3</v>
+        <v>K0103009800685,SASTH46,ANDYKA PUTRA PRASETYA,(XII TJKT 3),K0103009800685@gmail.com,XII TJKT 3</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
         <v>327</v>
       </c>
-      <c r="B70" s="2" t="s">
+      <c r="B70" t="s">
         <v>760</v>
       </c>
       <c r="C70" s="1" t="s">
@@ -4858,14 +4863,14 @@
       </c>
       <c r="G70" t="str">
         <f t="shared" si="1"/>
-        <v>K0103009800694,SASTH46@,ANIS TIARAWATI,(XII TJKT 3),K0103009800694@gmail.com,XII TJKT 3</v>
+        <v>K0103009800694,SASTH46,ANIS TIARAWATI,(XII TJKT 3),K0103009800694@gmail.com,XII TJKT 3</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
         <v>328</v>
       </c>
-      <c r="B71" s="2" t="s">
+      <c r="B71" t="s">
         <v>760</v>
       </c>
       <c r="C71" s="1" t="s">
@@ -4882,14 +4887,14 @@
       </c>
       <c r="G71" t="str">
         <f t="shared" si="1"/>
-        <v>K0103009800703,SASTH46@,ARMANDA PUTRA,(XII TJKT 3),K0103009800703@gmail.com,XII TJKT 3</v>
+        <v>K0103009800703,SASTH46,ARMANDA PUTRA,(XII TJKT 3),K0103009800703@gmail.com,XII TJKT 3</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
         <v>329</v>
       </c>
-      <c r="B72" s="2" t="s">
+      <c r="B72" t="s">
         <v>760</v>
       </c>
       <c r="C72" s="1" t="s">
@@ -4906,14 +4911,14 @@
       </c>
       <c r="G72" t="str">
         <f t="shared" si="1"/>
-        <v>K0103009800712,SASTH46@,CHANDRA ANDIKA,(XII TJKT 3),K0103009800712@gmail.com,XII TJKT 3</v>
+        <v>K0103009800712,SASTH46,CHANDRA ANDIKA,(XII TJKT 3),K0103009800712@gmail.com,XII TJKT 3</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
         <v>330</v>
       </c>
-      <c r="B73" s="2" t="s">
+      <c r="B73" t="s">
         <v>760</v>
       </c>
       <c r="C73" s="1" t="s">
@@ -4930,14 +4935,14 @@
       </c>
       <c r="G73" t="str">
         <f t="shared" si="1"/>
-        <v>K0103009800729,SASTH46@,DAVI TRISNA PRASETYA,(XII TJKT 3),K0103009800729@gmail.com,XII TJKT 3</v>
+        <v>K0103009800729,SASTH46,DAVI TRISNA PRASETYA,(XII TJKT 3),K0103009800729@gmail.com,XII TJKT 3</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
         <v>331</v>
       </c>
-      <c r="B74" s="2" t="s">
+      <c r="B74" t="s">
         <v>760</v>
       </c>
       <c r="C74" s="1" t="s">
@@ -4954,14 +4959,14 @@
       </c>
       <c r="G74" t="str">
         <f t="shared" si="1"/>
-        <v>K0103009800738,SASTH46@,DAVID HERMANSYAH,(XII TJKT 3),K0103009800738@gmail.com,XII TJKT 3</v>
+        <v>K0103009800738,SASTH46,DAVID HERMANSYAH,(XII TJKT 3),K0103009800738@gmail.com,XII TJKT 3</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
         <v>332</v>
       </c>
-      <c r="B75" s="2" t="s">
+      <c r="B75" t="s">
         <v>760</v>
       </c>
       <c r="C75" s="1" t="s">
@@ -4978,14 +4983,14 @@
       </c>
       <c r="G75" t="str">
         <f t="shared" si="1"/>
-        <v>K0103009800747,SASTH46@,DIAH SINTIA,(XII TJKT 3),K0103009800747@gmail.com,XII TJKT 3</v>
+        <v>K0103009800747,SASTH46,DIAH SINTIA,(XII TJKT 3),K0103009800747@gmail.com,XII TJKT 3</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
         <v>333</v>
       </c>
-      <c r="B76" s="2" t="s">
+      <c r="B76" t="s">
         <v>760</v>
       </c>
       <c r="C76" s="1" t="s">
@@ -5002,14 +5007,14 @@
       </c>
       <c r="G76" t="str">
         <f t="shared" si="1"/>
-        <v>K0103009800756,SASTH46@,FABRIAN AFRIANSYAH,(XII TJKT 3),K0103009800756@gmail.com,XII TJKT 3</v>
+        <v>K0103009800756,SASTH46,FABRIAN AFRIANSYAH,(XII TJKT 3),K0103009800756@gmail.com,XII TJKT 3</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
         <v>334</v>
       </c>
-      <c r="B77" s="2" t="s">
+      <c r="B77" t="s">
         <v>760</v>
       </c>
       <c r="C77" s="1" t="s">
@@ -5026,14 +5031,14 @@
       </c>
       <c r="G77" t="str">
         <f t="shared" si="1"/>
-        <v>K0103009800765,SASTH46@,FARIJ ASHIDIQI,(XII TJKT 3),K0103009800765@gmail.com,XII TJKT 3</v>
+        <v>K0103009800765,SASTH46,FARIJ ASHIDIQI,(XII TJKT 3),K0103009800765@gmail.com,XII TJKT 3</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
         <v>335</v>
       </c>
-      <c r="B78" s="2" t="s">
+      <c r="B78" t="s">
         <v>760</v>
       </c>
       <c r="C78" s="1" t="s">
@@ -5050,14 +5055,14 @@
       </c>
       <c r="G78" t="str">
         <f t="shared" si="1"/>
-        <v>K0103009800774,SASTH46@,FELIX ADIKA,(XII TJKT 3),K0103009800774@gmail.com,XII TJKT 3</v>
+        <v>K0103009800774,SASTH46,FELIX ADIKA,(XII TJKT 3),K0103009800774@gmail.com,XII TJKT 3</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
         <v>336</v>
       </c>
-      <c r="B79" s="2" t="s">
+      <c r="B79" t="s">
         <v>760</v>
       </c>
       <c r="C79" s="1" t="s">
@@ -5074,14 +5079,14 @@
       </c>
       <c r="G79" t="str">
         <f t="shared" si="1"/>
-        <v>K0103009800783,SASTH46@,FICRI CHOIRUL IMAM,(XII TJKT 3),K0103009800783@gmail.com,XII TJKT 3</v>
+        <v>K0103009800783,SASTH46,FICRI CHOIRUL IMAM,(XII TJKT 3),K0103009800783@gmail.com,XII TJKT 3</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
         <v>337</v>
       </c>
-      <c r="B80" s="2" t="s">
+      <c r="B80" t="s">
         <v>760</v>
       </c>
       <c r="C80" s="1" t="s">
@@ -5098,14 +5103,14 @@
       </c>
       <c r="G80" t="str">
         <f t="shared" si="1"/>
-        <v>K0103009800792,SASTH46@,FIRGIE HAFIANSYAH FAHREVI,(XII TJKT 3),K0103009800792@gmail.com,XII TJKT 3</v>
+        <v>K0103009800792,SASTH46,FIRGIE HAFIANSYAH FAHREVI,(XII TJKT 3),K0103009800792@gmail.com,XII TJKT 3</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
         <v>338</v>
       </c>
-      <c r="B81" s="2" t="s">
+      <c r="B81" t="s">
         <v>760</v>
       </c>
       <c r="C81" s="1" t="s">
@@ -5122,14 +5127,14 @@
       </c>
       <c r="G81" t="str">
         <f t="shared" si="1"/>
-        <v>K0103009800809,SASTH46@,GAFARA EKA FAHRIZA,(XII TJKT 3),K0103009800809@gmail.com,XII TJKT 3</v>
+        <v>K0103009800809,SASTH46,GAFARA EKA FAHRIZA,(XII TJKT 3),K0103009800809@gmail.com,XII TJKT 3</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
         <v>339</v>
       </c>
-      <c r="B82" s="2" t="s">
+      <c r="B82" t="s">
         <v>760</v>
       </c>
       <c r="C82" s="1" t="s">
@@ -5146,14 +5151,14 @@
       </c>
       <c r="G82" t="str">
         <f t="shared" si="1"/>
-        <v>K0103009800818,SASTH46@,GHUFRON KHAIRULLAH,(XII TJKT 3),K0103009800818@gmail.com,XII TJKT 3</v>
+        <v>K0103009800818,SASTH46,GHUFRON KHAIRULLAH,(XII TJKT 3),K0103009800818@gmail.com,XII TJKT 3</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
         <v>340</v>
       </c>
-      <c r="B83" s="2" t="s">
+      <c r="B83" t="s">
         <v>760</v>
       </c>
       <c r="C83" s="1" t="s">
@@ -5170,14 +5175,14 @@
       </c>
       <c r="G83" t="str">
         <f t="shared" si="1"/>
-        <v>K0103009800827,SASTH46@,KHARENAL ARDIANTONY,(XII TJKT 3),K0103009800827@gmail.com,XII TJKT 3</v>
+        <v>K0103009800827,SASTH46,KHARENAL ARDIANTONY,(XII TJKT 3),K0103009800827@gmail.com,XII TJKT 3</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
         <v>341</v>
       </c>
-      <c r="B84" s="2" t="s">
+      <c r="B84" t="s">
         <v>760</v>
       </c>
       <c r="C84" s="1" t="s">
@@ -5194,14 +5199,14 @@
       </c>
       <c r="G84" t="str">
         <f t="shared" si="1"/>
-        <v>K0103009800836,SASTH46@,MUHAMAD APRIANSYAH,(XII TJKT 3),K0103009800836@gmail.com,XII TJKT 3</v>
+        <v>K0103009800836,SASTH46,MUHAMAD APRIANSYAH,(XII TJKT 3),K0103009800836@gmail.com,XII TJKT 3</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
         <v>342</v>
       </c>
-      <c r="B85" s="2" t="s">
+      <c r="B85" t="s">
         <v>760</v>
       </c>
       <c r="C85" s="1" t="s">
@@ -5218,14 +5223,14 @@
       </c>
       <c r="G85" t="str">
         <f t="shared" si="1"/>
-        <v>K0103009800845,SASTH46@,MUHAMAD CHAIRIEL,(XII TJKT 3),K0103009800845@gmail.com,XII TJKT 3</v>
+        <v>K0103009800845,SASTH46,MUHAMAD CHAIRIEL,(XII TJKT 3),K0103009800845@gmail.com,XII TJKT 3</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
         <v>343</v>
       </c>
-      <c r="B86" s="2" t="s">
+      <c r="B86" t="s">
         <v>760</v>
       </c>
       <c r="C86" s="1" t="s">
@@ -5242,14 +5247,14 @@
       </c>
       <c r="G86" t="str">
         <f t="shared" si="1"/>
-        <v>K0103009800854,SASTH46@,MUHAMAD RIZKY,(XII TJKT 3),K0103009800854@gmail.com,XII TJKT 3</v>
+        <v>K0103009800854,SASTH46,MUHAMAD RIZKY,(XII TJKT 3),K0103009800854@gmail.com,XII TJKT 3</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
         <v>344</v>
       </c>
-      <c r="B87" s="2" t="s">
+      <c r="B87" t="s">
         <v>760</v>
       </c>
       <c r="C87" s="1" t="s">
@@ -5266,14 +5271,14 @@
       </c>
       <c r="G87" t="str">
         <f t="shared" si="1"/>
-        <v>K0103009800863,SASTH46@,MUHAMAD RIZKY FARIZAH,(XII TJKT 3),K0103009800863@gmail.com,XII TJKT 3</v>
+        <v>K0103009800863,SASTH46,MUHAMAD RIZKY FARIZAH,(XII TJKT 3),K0103009800863@gmail.com,XII TJKT 3</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
         <v>345</v>
       </c>
-      <c r="B88" s="2" t="s">
+      <c r="B88" t="s">
         <v>760</v>
       </c>
       <c r="C88" s="1" t="s">
@@ -5290,14 +5295,14 @@
       </c>
       <c r="G88" t="str">
         <f t="shared" si="1"/>
-        <v>K0103009800872,SASTH46@,MUHAMMAD AFDANY PUTRA WIJAYA,(XII TJKT 3),K0103009800872@gmail.com,XII TJKT 3</v>
+        <v>K0103009800872,SASTH46,MUHAMMAD AFDANY PUTRA WIJAYA,(XII TJKT 3),K0103009800872@gmail.com,XII TJKT 3</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
         <v>346</v>
       </c>
-      <c r="B89" s="2" t="s">
+      <c r="B89" t="s">
         <v>760</v>
       </c>
       <c r="C89" s="1" t="s">
@@ -5314,14 +5319,14 @@
       </c>
       <c r="G89" t="str">
         <f t="shared" si="1"/>
-        <v>K0103009800889,SASTH46@,MUHAMMAD ALFARIZA,(XII TJKT 3),K0103009800889@gmail.com,XII TJKT 3</v>
+        <v>K0103009800889,SASTH46,MUHAMMAD ALFARIZA,(XII TJKT 3),K0103009800889@gmail.com,XII TJKT 3</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
         <v>347</v>
       </c>
-      <c r="B90" s="2" t="s">
+      <c r="B90" t="s">
         <v>760</v>
       </c>
       <c r="C90" s="1" t="s">
@@ -5338,14 +5343,14 @@
       </c>
       <c r="G90" t="str">
         <f t="shared" si="1"/>
-        <v>K0103009800898,SASTH46@,MUHAMMAD REZA BAGUS SAPUTRA,(XII TJKT 3),K0103009800898@gmail.com,XII TJKT 3</v>
+        <v>K0103009800898,SASTH46,MUHAMMAD REZA BAGUS SAPUTRA,(XII TJKT 3),K0103009800898@gmail.com,XII TJKT 3</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
         <v>348</v>
       </c>
-      <c r="B91" s="2" t="s">
+      <c r="B91" t="s">
         <v>760</v>
       </c>
       <c r="C91" s="1" t="s">
@@ -5362,14 +5367,14 @@
       </c>
       <c r="G91" t="str">
         <f t="shared" si="1"/>
-        <v>K0103009800907,SASTH46@,MUHAMMAD RISKY,(XII TJKT 3),K0103009800907@gmail.com,XII TJKT 3</v>
+        <v>K0103009800907,SASTH46,MUHAMMAD RISKY,(XII TJKT 3),K0103009800907@gmail.com,XII TJKT 3</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
         <v>349</v>
       </c>
-      <c r="B92" s="2" t="s">
+      <c r="B92" t="s">
         <v>760</v>
       </c>
       <c r="C92" s="1" t="s">
@@ -5386,14 +5391,14 @@
       </c>
       <c r="G92" t="str">
         <f t="shared" si="1"/>
-        <v>K0103009800916,SASTH46@,NOVALLINO,(XII TJKT 3),K0103009800916@gmail.com,XII TJKT 3</v>
+        <v>K0103009800916,SASTH46,NOVALLINO,(XII TJKT 3),K0103009800916@gmail.com,XII TJKT 3</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
         <v>350</v>
       </c>
-      <c r="B93" s="2" t="s">
+      <c r="B93" t="s">
         <v>760</v>
       </c>
       <c r="C93" s="1" t="s">
@@ -5410,14 +5415,14 @@
       </c>
       <c r="G93" t="str">
         <f t="shared" si="1"/>
-        <v>K0103009800925,SASTH46@,RAFLY RAMADHAN LESMANA,(XII TJKT 3),K0103009800925@gmail.com,XII TJKT 3</v>
+        <v>K0103009800925,SASTH46,RAFLY RAMADHAN LESMANA,(XII TJKT 3),K0103009800925@gmail.com,XII TJKT 3</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
         <v>351</v>
       </c>
-      <c r="B94" s="2" t="s">
+      <c r="B94" t="s">
         <v>760</v>
       </c>
       <c r="C94" s="1" t="s">
@@ -5434,14 +5439,14 @@
       </c>
       <c r="G94" t="str">
         <f t="shared" si="1"/>
-        <v>K0103009800934,SASTH46@,RIFQI FADILLA DWIKA,(XII TJKT 3),K0103009800934@gmail.com,XII TJKT 3</v>
+        <v>K0103009800934,SASTH46,RIFQI FADILLA DWIKA,(XII TJKT 3),K0103009800934@gmail.com,XII TJKT 3</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
         <v>352</v>
       </c>
-      <c r="B95" s="2" t="s">
+      <c r="B95" t="s">
         <v>760</v>
       </c>
       <c r="C95" s="1" t="s">
@@ -5458,14 +5463,14 @@
       </c>
       <c r="G95" t="str">
         <f t="shared" si="1"/>
-        <v>K0103009800943,SASTH46@,RISVAL ANGGRA RESTA,(XII TJKT 3),K0103009800943@gmail.com,XII TJKT 3</v>
+        <v>K0103009800943,SASTH46,RISVAL ANGGRA RESTA,(XII TJKT 3),K0103009800943@gmail.com,XII TJKT 3</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
         <v>353</v>
       </c>
-      <c r="B96" s="2" t="s">
+      <c r="B96" t="s">
         <v>760</v>
       </c>
       <c r="C96" s="1" t="s">
@@ -5482,14 +5487,14 @@
       </c>
       <c r="G96" t="str">
         <f t="shared" si="1"/>
-        <v>K0103009800952,SASTH46@,SANDY PUTRA,(XII TJKT 3),K0103009800952@gmail.com,XII TJKT 3</v>
+        <v>K0103009800952,SASTH46,SANDY PUTRA,(XII TJKT 3),K0103009800952@gmail.com,XII TJKT 3</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
         <v>354</v>
       </c>
-      <c r="B97" s="2" t="s">
+      <c r="B97" t="s">
         <v>760</v>
       </c>
       <c r="C97" s="1" t="s">
@@ -5506,14 +5511,14 @@
       </c>
       <c r="G97" t="str">
         <f t="shared" si="1"/>
-        <v>K0103009800969,SASTH46@,SYAHRIL SUGANDA SAPUTRA,(XII TJKT 3),K0103009800969@gmail.com,XII TJKT 3</v>
+        <v>K0103009800969,SASTH46,SYAHRIL SUGANDA SAPUTRA,(XII TJKT 3),K0103009800969@gmail.com,XII TJKT 3</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
         <v>355</v>
       </c>
-      <c r="B98" s="2" t="s">
+      <c r="B98" t="s">
         <v>760</v>
       </c>
       <c r="C98" s="1" t="s">
@@ -5530,14 +5535,14 @@
       </c>
       <c r="G98" t="str">
         <f t="shared" si="1"/>
-        <v>K0103009800978,SASTH46@,TUBAGUS ABU BAKAR ZEIN,(XII TJKT 3),K0103009800978@gmail.com,XII TJKT 3</v>
+        <v>K0103009800978,SASTH46,TUBAGUS ABU BAKAR ZEIN,(XII TJKT 3),K0103009800978@gmail.com,XII TJKT 3</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
         <v>356</v>
       </c>
-      <c r="B99" s="2" t="s">
+      <c r="B99" t="s">
         <v>760</v>
       </c>
       <c r="C99" s="1" t="s">
@@ -5554,14 +5559,14 @@
       </c>
       <c r="G99" t="str">
         <f t="shared" si="1"/>
-        <v>K0103009800987,SASTH46@,ADITYA NURUL FIKRI,(XII AKL 1),K0103009800987@gmail.com,XII AKL 1</v>
+        <v>K0103009800987,SASTH46,ADITYA NURUL FIKRI,(XII AKL 1),K0103009800987@gmail.com,XII AKL 1</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
         <v>357</v>
       </c>
-      <c r="B100" s="2" t="s">
+      <c r="B100" t="s">
         <v>760</v>
       </c>
       <c r="C100" s="1" t="s">
@@ -5578,14 +5583,14 @@
       </c>
       <c r="G100" t="str">
         <f t="shared" si="1"/>
-        <v>K0103009800996,SASTH46@,ALIYA INDRIYANI PUTRI,(XII AKL 1),K0103009800996@gmail.com,XII AKL 1</v>
+        <v>K0103009800996,SASTH46,ALIYA INDRIYANI PUTRI,(XII AKL 1),K0103009800996@gmail.com,XII AKL 1</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
         <v>358</v>
       </c>
-      <c r="B101" s="2" t="s">
+      <c r="B101" t="s">
         <v>760</v>
       </c>
       <c r="C101" s="1" t="s">
@@ -5602,14 +5607,14 @@
       </c>
       <c r="G101" t="str">
         <f t="shared" si="1"/>
-        <v>K0103009801005,SASTH46@,ALYA NASYWA KHAERANI,(XII AKL 1),K0103009801005@gmail.com,XII AKL 1</v>
+        <v>K0103009801005,SASTH46,ALYA NASYWA KHAERANI,(XII AKL 1),K0103009801005@gmail.com,XII AKL 1</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
         <v>359</v>
       </c>
-      <c r="B102" s="2" t="s">
+      <c r="B102" t="s">
         <v>760</v>
       </c>
       <c r="C102" s="1" t="s">
@@ -5626,14 +5631,14 @@
       </c>
       <c r="G102" t="str">
         <f t="shared" si="1"/>
-        <v>K0103009801014,SASTH46@,AMRAN DANY,(XII AKL 1),K0103009801014@gmail.com,XII AKL 1</v>
+        <v>K0103009801014,SASTH46,AMRAN DANY,(XII AKL 1),K0103009801014@gmail.com,XII AKL 1</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
         <v>360</v>
       </c>
-      <c r="B103" s="2" t="s">
+      <c r="B103" t="s">
         <v>760</v>
       </c>
       <c r="C103" s="1" t="s">
@@ -5650,14 +5655,14 @@
       </c>
       <c r="G103" t="str">
         <f t="shared" si="1"/>
-        <v>K0103009801023,SASTH46@,BAGUS ARIEF SAPUTRA,(XII AKL 1),K0103009801023@gmail.com,XII AKL 1</v>
+        <v>K0103009801023,SASTH46,BAGUS ARIEF SAPUTRA,(XII AKL 1),K0103009801023@gmail.com,XII AKL 1</v>
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
         <v>361</v>
       </c>
-      <c r="B104" s="2" t="s">
+      <c r="B104" t="s">
         <v>760</v>
       </c>
       <c r="C104" s="1" t="s">
@@ -5674,14 +5679,14 @@
       </c>
       <c r="G104" t="str">
         <f t="shared" si="1"/>
-        <v>K0103009801032,SASTH46@,CATERINE NATALIA TEJA,(XII AKL 1),K0103009801032@gmail.com,XII AKL 1</v>
+        <v>K0103009801032,SASTH46,CATERINE NATALIA TEJA,(XII AKL 1),K0103009801032@gmail.com,XII AKL 1</v>
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
         <v>362</v>
       </c>
-      <c r="B105" s="2" t="s">
+      <c r="B105" t="s">
         <v>760</v>
       </c>
       <c r="C105" s="1" t="s">
@@ -5698,14 +5703,14 @@
       </c>
       <c r="G105" t="str">
         <f t="shared" si="1"/>
-        <v>K0103009801049,SASTH46@,CICI HERDIANTI,(XII AKL 1),K0103009801049@gmail.com,XII AKL 1</v>
+        <v>K0103009801049,SASTH46,CICI HERDIANTI,(XII AKL 1),K0103009801049@gmail.com,XII AKL 1</v>
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
         <v>363</v>
       </c>
-      <c r="B106" s="2" t="s">
+      <c r="B106" t="s">
         <v>760</v>
       </c>
       <c r="C106" s="1" t="s">
@@ -5722,14 +5727,14 @@
       </c>
       <c r="G106" t="str">
         <f t="shared" si="1"/>
-        <v>K0103009801058,SASTH46@,DAVID UMAR HAMZAH,(XII AKL 1),K0103009801058@gmail.com,XII AKL 1</v>
+        <v>K0103009801058,SASTH46,DAVID UMAR HAMZAH,(XII AKL 1),K0103009801058@gmail.com,XII AKL 1</v>
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="s">
         <v>364</v>
       </c>
-      <c r="B107" s="2" t="s">
+      <c r="B107" t="s">
         <v>760</v>
       </c>
       <c r="C107" s="1" t="s">
@@ -5746,14 +5751,14 @@
       </c>
       <c r="G107" t="str">
         <f t="shared" si="1"/>
-        <v>K0103009801067,SASTH46@,DHEASY NOVITA KUSUMA YETI,(XII AKL 1),K0103009801067@gmail.com,XII AKL 1</v>
+        <v>K0103009801067,SASTH46,DHEASY NOVITA KUSUMA YETI,(XII AKL 1),K0103009801067@gmail.com,XII AKL 1</v>
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
         <v>365</v>
       </c>
-      <c r="B108" s="2" t="s">
+      <c r="B108" t="s">
         <v>760</v>
       </c>
       <c r="C108" s="1" t="s">
@@ -5770,14 +5775,14 @@
       </c>
       <c r="G108" t="str">
         <f t="shared" si="1"/>
-        <v>K0103009801076,SASTH46@,FERI HIRAWAN,(XII AKL 1),K0103009801076@gmail.com,XII AKL 1</v>
+        <v>K0103009801076,SASTH46,FERI HIRAWAN,(XII AKL 1),K0103009801076@gmail.com,XII AKL 1</v>
       </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
         <v>366</v>
       </c>
-      <c r="B109" s="2" t="s">
+      <c r="B109" t="s">
         <v>760</v>
       </c>
       <c r="C109" s="1" t="s">
@@ -5794,14 +5799,14 @@
       </c>
       <c r="G109" t="str">
         <f t="shared" si="1"/>
-        <v>K0103009801085,SASTH46@,INDI NOVI TRIANI,(XII AKL 1),K0103009801085@gmail.com,XII AKL 1</v>
+        <v>K0103009801085,SASTH46,INDI NOVI TRIANI,(XII AKL 1),K0103009801085@gmail.com,XII AKL 1</v>
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
         <v>367</v>
       </c>
-      <c r="B110" s="2" t="s">
+      <c r="B110" t="s">
         <v>760</v>
       </c>
       <c r="C110" s="1" t="s">
@@ -5818,14 +5823,14 @@
       </c>
       <c r="G110" t="str">
         <f t="shared" si="1"/>
-        <v>K0103009801094,SASTH46@,INTAN HESTIYANA,(XII AKL 1),K0103009801094@gmail.com,XII AKL 1</v>
+        <v>K0103009801094,SASTH46,INTAN HESTIYANA,(XII AKL 1),K0103009801094@gmail.com,XII AKL 1</v>
       </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="s">
         <v>368</v>
       </c>
-      <c r="B111" s="2" t="s">
+      <c r="B111" t="s">
         <v>760</v>
       </c>
       <c r="C111" s="1" t="s">
@@ -5842,14 +5847,14 @@
       </c>
       <c r="G111" t="str">
         <f t="shared" si="1"/>
-        <v>K0103009801103,SASTH46@,MARCEL EDHI SUTIKNA,(XII AKL 1),K0103009801103@gmail.com,XII AKL 1</v>
+        <v>K0103009801103,SASTH46,MARCEL EDHI SUTIKNA,(XII AKL 1),K0103009801103@gmail.com,XII AKL 1</v>
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A112" s="1" t="s">
         <v>369</v>
       </c>
-      <c r="B112" s="2" t="s">
+      <c r="B112" t="s">
         <v>760</v>
       </c>
       <c r="C112" s="1" t="s">
@@ -5866,14 +5871,14 @@
       </c>
       <c r="G112" t="str">
         <f t="shared" si="1"/>
-        <v>K0103009801112,SASTH46@,MUHAMMAD RIFQY SAPUTRA,(XII AKL 1),K0103009801112@gmail.com,XII AKL 1</v>
+        <v>K0103009801112,SASTH46,MUHAMMAD RIFQY SAPUTRA,(XII AKL 1),K0103009801112@gmail.com,XII AKL 1</v>
       </c>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A113" s="1" t="s">
         <v>370</v>
       </c>
-      <c r="B113" s="2" t="s">
+      <c r="B113" t="s">
         <v>760</v>
       </c>
       <c r="C113" s="1" t="s">
@@ -5890,14 +5895,14 @@
       </c>
       <c r="G113" t="str">
         <f t="shared" si="1"/>
-        <v>K0103009801129,SASTH46@,NABILAH INTAN NURAINI,(XII AKL 1),K0103009801129@gmail.com,XII AKL 1</v>
+        <v>K0103009801129,SASTH46,NABILAH INTAN NURAINI,(XII AKL 1),K0103009801129@gmail.com,XII AKL 1</v>
       </c>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A114" s="1" t="s">
         <v>371</v>
       </c>
-      <c r="B114" s="2" t="s">
+      <c r="B114" t="s">
         <v>760</v>
       </c>
       <c r="C114" s="1" t="s">
@@ -5914,14 +5919,14 @@
       </c>
       <c r="G114" t="str">
         <f t="shared" si="1"/>
-        <v>K0103009801138,SASTH46@,NAILATUSY ARIBAH TASIMA,(XII AKL 1),K0103009801138@gmail.com,XII AKL 1</v>
+        <v>K0103009801138,SASTH46,NAILATUSY ARIBAH TASIMA,(XII AKL 1),K0103009801138@gmail.com,XII AKL 1</v>
       </c>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="s">
         <v>372</v>
       </c>
-      <c r="B115" s="2" t="s">
+      <c r="B115" t="s">
         <v>760</v>
       </c>
       <c r="C115" s="1" t="s">
@@ -5938,14 +5943,14 @@
       </c>
       <c r="G115" t="str">
         <f t="shared" si="1"/>
-        <v>K0103009801147,SASTH46@,NATASYA ANANDA SANTOSO,(XII AKL 1),K0103009801147@gmail.com,XII AKL 1</v>
+        <v>K0103009801147,SASTH46,NATASYA ANANDA SANTOSO,(XII AKL 1),K0103009801147@gmail.com,XII AKL 1</v>
       </c>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A116" s="1" t="s">
         <v>373</v>
       </c>
-      <c r="B116" s="2" t="s">
+      <c r="B116" t="s">
         <v>760</v>
       </c>
       <c r="C116" s="1" t="s">
@@ -5962,14 +5967,14 @@
       </c>
       <c r="G116" t="str">
         <f t="shared" si="1"/>
-        <v>K0103009801156,SASTH46@,NAZWA AULIA SALSABILA,(XII AKL 1),K0103009801156@gmail.com,XII AKL 1</v>
+        <v>K0103009801156,SASTH46,NAZWA AULIA SALSABILA,(XII AKL 1),K0103009801156@gmail.com,XII AKL 1</v>
       </c>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="B117" s="2" t="s">
+      <c r="B117" t="s">
         <v>760</v>
       </c>
       <c r="C117" s="1" t="s">
@@ -5986,14 +5991,14 @@
       </c>
       <c r="G117" t="str">
         <f t="shared" si="1"/>
-        <v>K0103009801165,SASTH46@,NIDA KHOIRURRAHMAH,(XII AKL 1),K0103009801165@gmail.com,XII AKL 1</v>
+        <v>K0103009801165,SASTH46,NIDA KHOIRURRAHMAH,(XII AKL 1),K0103009801165@gmail.com,XII AKL 1</v>
       </c>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A118" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="B118" s="2" t="s">
+      <c r="B118" t="s">
         <v>760</v>
       </c>
       <c r="C118" s="1" t="s">
@@ -6010,14 +6015,14 @@
       </c>
       <c r="G118" t="str">
         <f t="shared" si="1"/>
-        <v>K0103009801174,SASTH46@,RAMANDA OKTAVIANI,(XII AKL 1),K0103009801174@gmail.com,XII AKL 1</v>
+        <v>K0103009801174,SASTH46,RAMANDA OKTAVIANI,(XII AKL 1),K0103009801174@gmail.com,XII AKL 1</v>
       </c>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A119" s="1" t="s">
         <v>376</v>
       </c>
-      <c r="B119" s="2" t="s">
+      <c r="B119" t="s">
         <v>760</v>
       </c>
       <c r="C119" s="1" t="s">
@@ -6034,14 +6039,14 @@
       </c>
       <c r="G119" t="str">
         <f t="shared" si="1"/>
-        <v>K0103009801183,SASTH46@,RAMDZAN MULIAWAN TRAH SAPUTRA,(XII AKL 1),K0103009801183@gmail.com,XII AKL 1</v>
+        <v>K0103009801183,SASTH46,RAMDZAN MULIAWAN TRAH SAPUTRA,(XII AKL 1),K0103009801183@gmail.com,XII AKL 1</v>
       </c>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="s">
         <v>377</v>
       </c>
-      <c r="B120" s="2" t="s">
+      <c r="B120" t="s">
         <v>760</v>
       </c>
       <c r="C120" s="1" t="s">
@@ -6058,14 +6063,14 @@
       </c>
       <c r="G120" t="str">
         <f t="shared" si="1"/>
-        <v>K0103009801192,SASTH46@,SADIAH,(XII AKL 1),K0103009801192@gmail.com,XII AKL 1</v>
+        <v>K0103009801192,SASTH46,SADIAH,(XII AKL 1),K0103009801192@gmail.com,XII AKL 1</v>
       </c>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A121" s="1" t="s">
         <v>378</v>
       </c>
-      <c r="B121" s="2" t="s">
+      <c r="B121" t="s">
         <v>760</v>
       </c>
       <c r="C121" s="1" t="s">
@@ -6082,14 +6087,14 @@
       </c>
       <c r="G121" t="str">
         <f t="shared" si="1"/>
-        <v>K0103009801209,SASTH46@,SHERREN FEBRIANY,(XII AKL 1),K0103009801209@gmail.com,XII AKL 1</v>
+        <v>K0103009801209,SASTH46,SHERREN FEBRIANY,(XII AKL 1),K0103009801209@gmail.com,XII AKL 1</v>
       </c>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A122" s="1" t="s">
         <v>379</v>
       </c>
-      <c r="B122" s="2" t="s">
+      <c r="B122" t="s">
         <v>760</v>
       </c>
       <c r="C122" s="1" t="s">
@@ -6106,14 +6111,14 @@
       </c>
       <c r="G122" t="str">
         <f t="shared" si="1"/>
-        <v>K0103009801218,SASTH46@,STEVANI PUTRI WIJAYA,(XII AKL 1),K0103009801218@gmail.com,XII AKL 1</v>
+        <v>K0103009801218,SASTH46,STEVANI PUTRI WIJAYA,(XII AKL 1),K0103009801218@gmail.com,XII AKL 1</v>
       </c>
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A123" s="1" t="s">
         <v>380</v>
       </c>
-      <c r="B123" s="2" t="s">
+      <c r="B123" t="s">
         <v>760</v>
       </c>
       <c r="C123" s="1" t="s">
@@ -6130,14 +6135,14 @@
       </c>
       <c r="G123" t="str">
         <f t="shared" si="1"/>
-        <v>K0103009801227,SASTH46@,VANI HARIYANTI,(XII AKL 1),K0103009801227@gmail.com,XII AKL 1</v>
+        <v>K0103009801227,SASTH46,VANI HARIYANTI,(XII AKL 1),K0103009801227@gmail.com,XII AKL 1</v>
       </c>
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A124" s="1" t="s">
         <v>381</v>
       </c>
-      <c r="B124" s="2" t="s">
+      <c r="B124" t="s">
         <v>760</v>
       </c>
       <c r="C124" s="1" t="s">
@@ -6154,14 +6159,14 @@
       </c>
       <c r="G124" t="str">
         <f t="shared" si="1"/>
-        <v>K0103009801236,SASTH46@,ADITYA PRATAMA,(XII AKL 2),K0103009801236@gmail.com,XII AKL 2</v>
+        <v>K0103009801236,SASTH46,ADITYA PRATAMA,(XII AKL 2),K0103009801236@gmail.com,XII AKL 2</v>
       </c>
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A125" s="1" t="s">
         <v>382</v>
       </c>
-      <c r="B125" s="2" t="s">
+      <c r="B125" t="s">
         <v>760</v>
       </c>
       <c r="C125" s="1" t="s">
@@ -6178,14 +6183,14 @@
       </c>
       <c r="G125" t="str">
         <f t="shared" si="1"/>
-        <v>K0103009801245,SASTH46@,ADUTA BAYHAQI,(XII AKL 2),K0103009801245@gmail.com,XII AKL 2</v>
+        <v>K0103009801245,SASTH46,ADUTA BAYHAQI,(XII AKL 2),K0103009801245@gmail.com,XII AKL 2</v>
       </c>
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A126" s="1" t="s">
         <v>383</v>
       </c>
-      <c r="B126" s="2" t="s">
+      <c r="B126" t="s">
         <v>760</v>
       </c>
       <c r="C126" s="1" t="s">
@@ -6202,14 +6207,14 @@
       </c>
       <c r="G126" t="str">
         <f t="shared" si="1"/>
-        <v>K0103009801254,SASTH46@,AHMAD RIDWAN,(XII AKL 2),K0103009801254@gmail.com,XII AKL 2</v>
+        <v>K0103009801254,SASTH46,AHMAD RIDWAN,(XII AKL 2),K0103009801254@gmail.com,XII AKL 2</v>
       </c>
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A127" s="1" t="s">
         <v>384</v>
       </c>
-      <c r="B127" s="2" t="s">
+      <c r="B127" t="s">
         <v>760</v>
       </c>
       <c r="C127" s="1" t="s">
@@ -6226,14 +6231,14 @@
       </c>
       <c r="G127" t="str">
         <f t="shared" si="1"/>
-        <v>K0103009801263,SASTH46@,ANIN DWI RAHMAWATI,(XII AKL 2),K0103009801263@gmail.com,XII AKL 2</v>
+        <v>K0103009801263,SASTH46,ANIN DWI RAHMAWATI,(XII AKL 2),K0103009801263@gmail.com,XII AKL 2</v>
       </c>
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A128" s="1" t="s">
         <v>385</v>
       </c>
-      <c r="B128" s="2" t="s">
+      <c r="B128" t="s">
         <v>760</v>
       </c>
       <c r="C128" s="1" t="s">
@@ -6250,14 +6255,14 @@
       </c>
       <c r="G128" t="str">
         <f t="shared" si="1"/>
-        <v>K0103009801272,SASTH46@,AULIA DZURUN NAFIS,(XII AKL 2),K0103009801272@gmail.com,XII AKL 2</v>
+        <v>K0103009801272,SASTH46,AULIA DZURUN NAFIS,(XII AKL 2),K0103009801272@gmail.com,XII AKL 2</v>
       </c>
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A129" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="B129" s="2" t="s">
+      <c r="B129" t="s">
         <v>760</v>
       </c>
       <c r="C129" s="1" t="s">
@@ -6274,14 +6279,14 @@
       </c>
       <c r="G129" t="str">
         <f t="shared" si="1"/>
-        <v>K0103009801289,SASTH46@,CHERRYL DEANDYA KHALISHAH,(XII AKL 2),K0103009801289@gmail.com,XII AKL 2</v>
+        <v>K0103009801289,SASTH46,CHERRYL DEANDYA KHALISHAH,(XII AKL 2),K0103009801289@gmail.com,XII AKL 2</v>
       </c>
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A130" s="1" t="s">
         <v>387</v>
       </c>
-      <c r="B130" s="2" t="s">
+      <c r="B130" t="s">
         <v>760</v>
       </c>
       <c r="C130" s="1" t="s">
@@ -6298,14 +6303,14 @@
       </c>
       <c r="G130" t="str">
         <f t="shared" ref="G130:G193" si="2">CONCATENATE(A130,",",B130,",",C130,",",D130,",",E130,",",F130)</f>
-        <v>K0103009801298,SASTH46@,DEWI PURNAMA SARI,(XII AKL 2),K0103009801298@gmail.com,XII AKL 2</v>
+        <v>K0103009801298,SASTH46,DEWI PURNAMA SARI,(XII AKL 2),K0103009801298@gmail.com,XII AKL 2</v>
       </c>
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A131" s="1" t="s">
         <v>388</v>
       </c>
-      <c r="B131" s="2" t="s">
+      <c r="B131" t="s">
         <v>760</v>
       </c>
       <c r="C131" s="1" t="s">
@@ -6322,14 +6327,14 @@
       </c>
       <c r="G131" t="str">
         <f t="shared" si="2"/>
-        <v>K0103009801307,SASTH46@,DWI PRAMBANDARI,(XII AKL 2),K0103009801307@gmail.com,XII AKL 2</v>
+        <v>K0103009801307,SASTH46,DWI PRAMBANDARI,(XII AKL 2),K0103009801307@gmail.com,XII AKL 2</v>
       </c>
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A132" s="1" t="s">
         <v>389</v>
       </c>
-      <c r="B132" s="2" t="s">
+      <c r="B132" t="s">
         <v>760</v>
       </c>
       <c r="C132" s="1" t="s">
@@ -6346,14 +6351,14 @@
       </c>
       <c r="G132" t="str">
         <f t="shared" si="2"/>
-        <v>K0103009801316,SASTH46@,ERIKA ILMANISA,(XII AKL 2),K0103009801316@gmail.com,XII AKL 2</v>
+        <v>K0103009801316,SASTH46,ERIKA ILMANISA,(XII AKL 2),K0103009801316@gmail.com,XII AKL 2</v>
       </c>
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A133" s="1" t="s">
         <v>390</v>
       </c>
-      <c r="B133" s="2" t="s">
+      <c r="B133" t="s">
         <v>760</v>
       </c>
       <c r="C133" s="1" t="s">
@@ -6370,14 +6375,14 @@
       </c>
       <c r="G133" t="str">
         <f t="shared" si="2"/>
-        <v>K0103009801325,SASTH46@,INEU SANTIKA,(XII AKL 2),K0103009801325@gmail.com,XII AKL 2</v>
+        <v>K0103009801325,SASTH46,INEU SANTIKA,(XII AKL 2),K0103009801325@gmail.com,XII AKL 2</v>
       </c>
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A134" s="1" t="s">
         <v>391</v>
       </c>
-      <c r="B134" s="2" t="s">
+      <c r="B134" t="s">
         <v>760</v>
       </c>
       <c r="C134" s="1" t="s">
@@ -6394,14 +6399,14 @@
       </c>
       <c r="G134" t="str">
         <f t="shared" si="2"/>
-        <v>K0103009801334,SASTH46@,IRWANSYAH,(XII AKL 2),K0103009801334@gmail.com,XII AKL 2</v>
+        <v>K0103009801334,SASTH46,IRWANSYAH,(XII AKL 2),K0103009801334@gmail.com,XII AKL 2</v>
       </c>
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A135" s="1" t="s">
         <v>392</v>
       </c>
-      <c r="B135" s="2" t="s">
+      <c r="B135" t="s">
         <v>760</v>
       </c>
       <c r="C135" s="1" t="s">
@@ -6418,14 +6423,14 @@
       </c>
       <c r="G135" t="str">
         <f t="shared" si="2"/>
-        <v>K0103009801343,SASTH46@,MUHAMMAD YUSUF FADLAN,(XII AKL 2),K0103009801343@gmail.com,XII AKL 2</v>
+        <v>K0103009801343,SASTH46,MUHAMMAD YUSUF FADLAN,(XII AKL 2),K0103009801343@gmail.com,XII AKL 2</v>
       </c>
     </row>
     <row r="136" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A136" s="1" t="s">
         <v>393</v>
       </c>
-      <c r="B136" s="2" t="s">
+      <c r="B136" t="s">
         <v>760</v>
       </c>
       <c r="C136" s="1" t="s">
@@ -6442,14 +6447,14 @@
       </c>
       <c r="G136" t="str">
         <f t="shared" si="2"/>
-        <v>K0103009801352,SASTH46@,NANDA AULYA ARIYANDI,(XII AKL 2),K0103009801352@gmail.com,XII AKL 2</v>
+        <v>K0103009801352,SASTH46,NANDA AULYA ARIYANDI,(XII AKL 2),K0103009801352@gmail.com,XII AKL 2</v>
       </c>
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A137" s="1" t="s">
         <v>394</v>
       </c>
-      <c r="B137" s="2" t="s">
+      <c r="B137" t="s">
         <v>760</v>
       </c>
       <c r="C137" s="1" t="s">
@@ -6466,14 +6471,14 @@
       </c>
       <c r="G137" t="str">
         <f t="shared" si="2"/>
-        <v>K0103009801369,SASTH46@,NAURAH SASMITA PUTRI,(XII AKL 2),K0103009801369@gmail.com,XII AKL 2</v>
+        <v>K0103009801369,SASTH46,NAURAH SASMITA PUTRI,(XII AKL 2),K0103009801369@gmail.com,XII AKL 2</v>
       </c>
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A138" s="1" t="s">
         <v>395</v>
       </c>
-      <c r="B138" s="2" t="s">
+      <c r="B138" t="s">
         <v>760</v>
       </c>
       <c r="C138" s="1" t="s">
@@ -6490,14 +6495,14 @@
       </c>
       <c r="G138" t="str">
         <f t="shared" si="2"/>
-        <v>K0103009801378,SASTH46@,NAYLA PUTRI RAHARI,(XII AKL 2),K0103009801378@gmail.com,XII AKL 2</v>
+        <v>K0103009801378,SASTH46,NAYLA PUTRI RAHARI,(XII AKL 2),K0103009801378@gmail.com,XII AKL 2</v>
       </c>
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A139" s="1" t="s">
         <v>396</v>
       </c>
-      <c r="B139" s="2" t="s">
+      <c r="B139" t="s">
         <v>760</v>
       </c>
       <c r="C139" s="1" t="s">
@@ -6514,14 +6519,14 @@
       </c>
       <c r="G139" t="str">
         <f t="shared" si="2"/>
-        <v>K0103009801387,SASTH46@,NISA UL HASANAH,(XII AKL 2),K0103009801387@gmail.com,XII AKL 2</v>
+        <v>K0103009801387,SASTH46,NISA UL HASANAH,(XII AKL 2),K0103009801387@gmail.com,XII AKL 2</v>
       </c>
     </row>
     <row r="140" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A140" s="1" t="s">
         <v>397</v>
       </c>
-      <c r="B140" s="2" t="s">
+      <c r="B140" t="s">
         <v>760</v>
       </c>
       <c r="C140" s="1" t="s">
@@ -6538,14 +6543,14 @@
       </c>
       <c r="G140" t="str">
         <f t="shared" si="2"/>
-        <v>K0103009801396,SASTH46@,ORYSA SATIVA,(XII AKL 2),K0103009801396@gmail.com,XII AKL 2</v>
+        <v>K0103009801396,SASTH46,ORYSA SATIVA,(XII AKL 2),K0103009801396@gmail.com,XII AKL 2</v>
       </c>
     </row>
     <row r="141" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A141" s="1" t="s">
         <v>398</v>
       </c>
-      <c r="B141" s="2" t="s">
+      <c r="B141" t="s">
         <v>760</v>
       </c>
       <c r="C141" s="1" t="s">
@@ -6562,14 +6567,14 @@
       </c>
       <c r="G141" t="str">
         <f t="shared" si="2"/>
-        <v>K0103009801405,SASTH46@,RIVAL WAHYUDIN,(XII AKL 2),K0103009801405@gmail.com,XII AKL 2</v>
+        <v>K0103009801405,SASTH46,RIVAL WAHYUDIN,(XII AKL 2),K0103009801405@gmail.com,XII AKL 2</v>
       </c>
     </row>
     <row r="142" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A142" s="1" t="s">
         <v>399</v>
       </c>
-      <c r="B142" s="2" t="s">
+      <c r="B142" t="s">
         <v>760</v>
       </c>
       <c r="C142" s="1" t="s">
@@ -6586,14 +6591,14 @@
       </c>
       <c r="G142" t="str">
         <f t="shared" si="2"/>
-        <v>K0103009801414,SASTH46@,RIZKY DWI KARNADI,(XII AKL 2),K0103009801414@gmail.com,XII AKL 2</v>
+        <v>K0103009801414,SASTH46,RIZKY DWI KARNADI,(XII AKL 2),K0103009801414@gmail.com,XII AKL 2</v>
       </c>
     </row>
     <row r="143" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A143" s="1" t="s">
         <v>400</v>
       </c>
-      <c r="B143" s="2" t="s">
+      <c r="B143" t="s">
         <v>760</v>
       </c>
       <c r="C143" s="1" t="s">
@@ -6610,14 +6615,14 @@
       </c>
       <c r="G143" t="str">
         <f t="shared" si="2"/>
-        <v>K0103009801423,SASTH46@,SARAH AULIYA,(XII AKL 2),K0103009801423@gmail.com,XII AKL 2</v>
+        <v>K0103009801423,SASTH46,SARAH AULIYA,(XII AKL 2),K0103009801423@gmail.com,XII AKL 2</v>
       </c>
     </row>
     <row r="144" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A144" s="1" t="s">
         <v>401</v>
       </c>
-      <c r="B144" s="2" t="s">
+      <c r="B144" t="s">
         <v>760</v>
       </c>
       <c r="C144" s="1" t="s">
@@ -6634,14 +6639,14 @@
       </c>
       <c r="G144" t="str">
         <f t="shared" si="2"/>
-        <v>K0103009801432,SASTH46@,SELO GIRI ADJI PANGESTU,(XII AKL 2),K0103009801432@gmail.com,XII AKL 2</v>
+        <v>K0103009801432,SASTH46,SELO GIRI ADJI PANGESTU,(XII AKL 2),K0103009801432@gmail.com,XII AKL 2</v>
       </c>
     </row>
     <row r="145" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A145" s="1" t="s">
         <v>402</v>
       </c>
-      <c r="B145" s="2" t="s">
+      <c r="B145" t="s">
         <v>760</v>
       </c>
       <c r="C145" s="1" t="s">
@@ -6658,14 +6663,14 @@
       </c>
       <c r="G145" t="str">
         <f t="shared" si="2"/>
-        <v>K0103009801449,SASTH46@,WULAN SUCI PUSPITASARI,(XII AKL 2),K0103009801449@gmail.com,XII AKL 2</v>
+        <v>K0103009801449,SASTH46,WULAN SUCI PUSPITASARI,(XII AKL 2),K0103009801449@gmail.com,XII AKL 2</v>
       </c>
     </row>
     <row r="146" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A146" s="1" t="s">
         <v>403</v>
       </c>
-      <c r="B146" s="2" t="s">
+      <c r="B146" t="s">
         <v>760</v>
       </c>
       <c r="C146" s="1" t="s">
@@ -6682,14 +6687,14 @@
       </c>
       <c r="G146" t="str">
         <f t="shared" si="2"/>
-        <v>K0103009801458,SASTH46@,WULAN TARI,(XII AKL 2),K0103009801458@gmail.com,XII AKL 2</v>
+        <v>K0103009801458,SASTH46,WULAN TARI,(XII AKL 2),K0103009801458@gmail.com,XII AKL 2</v>
       </c>
     </row>
     <row r="147" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A147" s="1" t="s">
         <v>404</v>
       </c>
-      <c r="B147" s="2" t="s">
+      <c r="B147" t="s">
         <v>760</v>
       </c>
       <c r="C147" s="1" t="s">
@@ -6706,14 +6711,14 @@
       </c>
       <c r="G147" t="str">
         <f t="shared" si="2"/>
-        <v>K0103009801467,SASTH46@,ADELIA ANGRAINI ZAHRA,(XII MPLB 1),K0103009801467@gmail.com,XII MPLB 1</v>
+        <v>K0103009801467,SASTH46,ADELIA ANGRAINI ZAHRA,(XII MPLB 1),K0103009801467@gmail.com,XII MPLB 1</v>
       </c>
     </row>
     <row r="148" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A148" s="1" t="s">
         <v>405</v>
       </c>
-      <c r="B148" s="2" t="s">
+      <c r="B148" t="s">
         <v>760</v>
       </c>
       <c r="C148" s="1" t="s">
@@ -6730,14 +6735,14 @@
       </c>
       <c r="G148" t="str">
         <f t="shared" si="2"/>
-        <v>K0103009801476,SASTH46@,AGNES PASKA TAMBUNAN,(XII MPLB 1),K0103009801476@gmail.com,XII MPLB 1</v>
+        <v>K0103009801476,SASTH46,AGNES PASKA TAMBUNAN,(XII MPLB 1),K0103009801476@gmail.com,XII MPLB 1</v>
       </c>
     </row>
     <row r="149" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A149" s="1" t="s">
         <v>406</v>
       </c>
-      <c r="B149" s="2" t="s">
+      <c r="B149" t="s">
         <v>760</v>
       </c>
       <c r="C149" s="1" t="s">
@@ -6754,14 +6759,14 @@
       </c>
       <c r="G149" t="str">
         <f t="shared" si="2"/>
-        <v>K0103009801485,SASTH46@,ALIVIA SUCI RAMADHANI,(XII MPLB 1),K0103009801485@gmail.com,XII MPLB 1</v>
+        <v>K0103009801485,SASTH46,ALIVIA SUCI RAMADHANI,(XII MPLB 1),K0103009801485@gmail.com,XII MPLB 1</v>
       </c>
     </row>
     <row r="150" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A150" s="1" t="s">
         <v>407</v>
       </c>
-      <c r="B150" s="2" t="s">
+      <c r="B150" t="s">
         <v>760</v>
       </c>
       <c r="C150" s="1" t="s">
@@ -6778,14 +6783,14 @@
       </c>
       <c r="G150" t="str">
         <f t="shared" si="2"/>
-        <v>K0103009801494,SASTH46@,AMANDA PUTRI SITIO,(XII MPLB 1),K0103009801494@gmail.com,XII MPLB 1</v>
+        <v>K0103009801494,SASTH46,AMANDA PUTRI SITIO,(XII MPLB 1),K0103009801494@gmail.com,XII MPLB 1</v>
       </c>
     </row>
     <row r="151" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A151" s="1" t="s">
         <v>408</v>
       </c>
-      <c r="B151" s="2" t="s">
+      <c r="B151" t="s">
         <v>760</v>
       </c>
       <c r="C151" s="1" t="s">
@@ -6802,14 +6807,14 @@
       </c>
       <c r="G151" t="str">
         <f t="shared" si="2"/>
-        <v>K0103009801503,SASTH46@,AMANDA YULIA PERMATA SARI,(XII MPLB 1),K0103009801503@gmail.com,XII MPLB 1</v>
+        <v>K0103009801503,SASTH46,AMANDA YULIA PERMATA SARI,(XII MPLB 1),K0103009801503@gmail.com,XII MPLB 1</v>
       </c>
     </row>
     <row r="152" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A152" s="1" t="s">
         <v>409</v>
       </c>
-      <c r="B152" s="2" t="s">
+      <c r="B152" t="s">
         <v>760</v>
       </c>
       <c r="C152" s="1" t="s">
@@ -6826,14 +6831,14 @@
       </c>
       <c r="G152" t="str">
         <f t="shared" si="2"/>
-        <v>K0103009801512,SASTH46@,AWALIA PUTRI,(XII MPLB 1),K0103009801512@gmail.com,XII MPLB 1</v>
+        <v>K0103009801512,SASTH46,AWALIA PUTRI,(XII MPLB 1),K0103009801512@gmail.com,XII MPLB 1</v>
       </c>
     </row>
     <row r="153" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A153" s="1" t="s">
         <v>410</v>
       </c>
-      <c r="B153" s="2" t="s">
+      <c r="B153" t="s">
         <v>760</v>
       </c>
       <c r="C153" s="1" t="s">
@@ -6850,14 +6855,14 @@
       </c>
       <c r="G153" t="str">
         <f t="shared" si="2"/>
-        <v>K0103009801529,SASTH46@,DELLY PUSPITA SARI,(XII MPLB 1),K0103009801529@gmail.com,XII MPLB 1</v>
+        <v>K0103009801529,SASTH46,DELLY PUSPITA SARI,(XII MPLB 1),K0103009801529@gmail.com,XII MPLB 1</v>
       </c>
     </row>
     <row r="154" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A154" s="1" t="s">
         <v>411</v>
       </c>
-      <c r="B154" s="2" t="s">
+      <c r="B154" t="s">
         <v>760</v>
       </c>
       <c r="C154" s="1" t="s">
@@ -6874,14 +6879,14 @@
       </c>
       <c r="G154" t="str">
         <f t="shared" si="2"/>
-        <v>K0103009801538,SASTH46@,DEWI SHINTA WIJAYA,(XII MPLB 1),K0103009801538@gmail.com,XII MPLB 1</v>
+        <v>K0103009801538,SASTH46,DEWI SHINTA WIJAYA,(XII MPLB 1),K0103009801538@gmail.com,XII MPLB 1</v>
       </c>
     </row>
     <row r="155" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A155" s="1" t="s">
         <v>412</v>
       </c>
-      <c r="B155" s="2" t="s">
+      <c r="B155" t="s">
         <v>760</v>
       </c>
       <c r="C155" s="1" t="s">
@@ -6898,14 +6903,14 @@
       </c>
       <c r="G155" t="str">
         <f t="shared" si="2"/>
-        <v>K0103009801547,SASTH46@,DIFA' AISYAH PUTRI,(XII MPLB 1),K0103009801547@gmail.com,XII MPLB 1</v>
+        <v>K0103009801547,SASTH46,DIFA' AISYAH PUTRI,(XII MPLB 1),K0103009801547@gmail.com,XII MPLB 1</v>
       </c>
     </row>
     <row r="156" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A156" s="1" t="s">
         <v>413</v>
       </c>
-      <c r="B156" s="2" t="s">
+      <c r="B156" t="s">
         <v>760</v>
       </c>
       <c r="C156" s="1" t="s">
@@ -6922,14 +6927,14 @@
       </c>
       <c r="G156" t="str">
         <f t="shared" si="2"/>
-        <v>K0103009801556,SASTH46@,DINDA SYAFITRI,(XII MPLB 1),K0103009801556@gmail.com,XII MPLB 1</v>
+        <v>K0103009801556,SASTH46,DINDA SYAFITRI,(XII MPLB 1),K0103009801556@gmail.com,XII MPLB 1</v>
       </c>
     </row>
     <row r="157" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A157" s="1" t="s">
         <v>414</v>
       </c>
-      <c r="B157" s="2" t="s">
+      <c r="B157" t="s">
         <v>760</v>
       </c>
       <c r="C157" s="1" t="s">
@@ -6946,14 +6951,14 @@
       </c>
       <c r="G157" t="str">
         <f t="shared" si="2"/>
-        <v>K0103009801565,SASTH46@,ELSA APRILIA SAFITRI,(XII MPLB 1),K0103009801565@gmail.com,XII MPLB 1</v>
+        <v>K0103009801565,SASTH46,ELSA APRILIA SAFITRI,(XII MPLB 1),K0103009801565@gmail.com,XII MPLB 1</v>
       </c>
     </row>
     <row r="158" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A158" s="1" t="s">
         <v>415</v>
       </c>
-      <c r="B158" s="2" t="s">
+      <c r="B158" t="s">
         <v>760</v>
       </c>
       <c r="C158" s="1" t="s">
@@ -6970,14 +6975,14 @@
       </c>
       <c r="G158" t="str">
         <f t="shared" si="2"/>
-        <v>K0103009801574,SASTH46@,FANNY DWI MUNAENI,(XII MPLB 1),K0103009801574@gmail.com,XII MPLB 1</v>
+        <v>K0103009801574,SASTH46,FANNY DWI MUNAENI,(XII MPLB 1),K0103009801574@gmail.com,XII MPLB 1</v>
       </c>
     </row>
     <row r="159" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A159" s="1" t="s">
         <v>416</v>
       </c>
-      <c r="B159" s="2" t="s">
+      <c r="B159" t="s">
         <v>760</v>
       </c>
       <c r="C159" s="1" t="s">
@@ -6994,14 +6999,14 @@
       </c>
       <c r="G159" t="str">
         <f t="shared" si="2"/>
-        <v>K0103009801583,SASTH46@,FRIDA SIWI MAYSAWATI,(XII MPLB 1),K0103009801583@gmail.com,XII MPLB 1</v>
+        <v>K0103009801583,SASTH46,FRIDA SIWI MAYSAWATI,(XII MPLB 1),K0103009801583@gmail.com,XII MPLB 1</v>
       </c>
     </row>
     <row r="160" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A160" s="1" t="s">
         <v>417</v>
       </c>
-      <c r="B160" s="2" t="s">
+      <c r="B160" t="s">
         <v>760</v>
       </c>
       <c r="C160" s="1" t="s">
@@ -7018,14 +7023,14 @@
       </c>
       <c r="G160" t="str">
         <f t="shared" si="2"/>
-        <v>K0103009801592,SASTH46@,HARTANTI WIJAYA,(XII MPLB 1),K0103009801592@gmail.com,XII MPLB 1</v>
+        <v>K0103009801592,SASTH46,HARTANTI WIJAYA,(XII MPLB 1),K0103009801592@gmail.com,XII MPLB 1</v>
       </c>
     </row>
     <row r="161" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A161" s="1" t="s">
         <v>418</v>
       </c>
-      <c r="B161" s="2" t="s">
+      <c r="B161" t="s">
         <v>760</v>
       </c>
       <c r="C161" s="1" t="s">
@@ -7042,14 +7047,14 @@
       </c>
       <c r="G161" t="str">
         <f t="shared" si="2"/>
-        <v>K0103009801609,SASTH46@,JESICA TRISIA PUTRI,(XII MPLB 1),K0103009801609@gmail.com,XII MPLB 1</v>
+        <v>K0103009801609,SASTH46,JESICA TRISIA PUTRI,(XII MPLB 1),K0103009801609@gmail.com,XII MPLB 1</v>
       </c>
     </row>
     <row r="162" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A162" s="1" t="s">
         <v>419</v>
       </c>
-      <c r="B162" s="2" t="s">
+      <c r="B162" t="s">
         <v>760</v>
       </c>
       <c r="C162" s="1" t="s">
@@ -7066,14 +7071,14 @@
       </c>
       <c r="G162" t="str">
         <f t="shared" si="2"/>
-        <v>K0103009801618,SASTH46@,KALISA NABILA,(XII MPLB 1),K0103009801618@gmail.com,XII MPLB 1</v>
+        <v>K0103009801618,SASTH46,KALISA NABILA,(XII MPLB 1),K0103009801618@gmail.com,XII MPLB 1</v>
       </c>
     </row>
     <row r="163" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A163" s="1" t="s">
         <v>420</v>
       </c>
-      <c r="B163" s="2" t="s">
+      <c r="B163" t="s">
         <v>760</v>
       </c>
       <c r="C163" s="1" t="s">
@@ -7090,14 +7095,14 @@
       </c>
       <c r="G163" t="str">
         <f t="shared" si="2"/>
-        <v>K0103009801627,SASTH46@,MARSELLINA,(XII MPLB 1),K0103009801627@gmail.com,XII MPLB 1</v>
+        <v>K0103009801627,SASTH46,MARSELLINA,(XII MPLB 1),K0103009801627@gmail.com,XII MPLB 1</v>
       </c>
     </row>
     <row r="164" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A164" s="1" t="s">
         <v>421</v>
       </c>
-      <c r="B164" s="2" t="s">
+      <c r="B164" t="s">
         <v>760</v>
       </c>
       <c r="C164" s="1" t="s">
@@ -7114,14 +7119,14 @@
       </c>
       <c r="G164" t="str">
         <f t="shared" si="2"/>
-        <v>K0103009801636,SASTH46@,MEI RIYANTI,(XII MPLB 1),K0103009801636@gmail.com,XII MPLB 1</v>
+        <v>K0103009801636,SASTH46,MEI RIYANTI,(XII MPLB 1),K0103009801636@gmail.com,XII MPLB 1</v>
       </c>
     </row>
     <row r="165" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A165" s="1" t="s">
         <v>422</v>
       </c>
-      <c r="B165" s="2" t="s">
+      <c r="B165" t="s">
         <v>760</v>
       </c>
       <c r="C165" s="1" t="s">
@@ -7138,14 +7143,14 @@
       </c>
       <c r="G165" t="str">
         <f t="shared" si="2"/>
-        <v>K0103009801645,SASTH46@,NABILA MUKHTAR,(XII MPLB 1),K0103009801645@gmail.com,XII MPLB 1</v>
+        <v>K0103009801645,SASTH46,NABILA MUKHTAR,(XII MPLB 1),K0103009801645@gmail.com,XII MPLB 1</v>
       </c>
     </row>
     <row r="166" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A166" s="1" t="s">
         <v>423</v>
       </c>
-      <c r="B166" s="2" t="s">
+      <c r="B166" t="s">
         <v>760</v>
       </c>
       <c r="C166" s="1" t="s">
@@ -7162,14 +7167,14 @@
       </c>
       <c r="G166" t="str">
         <f t="shared" si="2"/>
-        <v>K0103009801654,SASTH46@,NAGITA ZAHARANI,(XII MPLB 1),K0103009801654@gmail.com,XII MPLB 1</v>
+        <v>K0103009801654,SASTH46,NAGITA ZAHARANI,(XII MPLB 1),K0103009801654@gmail.com,XII MPLB 1</v>
       </c>
     </row>
     <row r="167" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A167" s="1" t="s">
         <v>424</v>
       </c>
-      <c r="B167" s="2" t="s">
+      <c r="B167" t="s">
         <v>760</v>
       </c>
       <c r="C167" s="1" t="s">
@@ -7186,14 +7191,14 @@
       </c>
       <c r="G167" t="str">
         <f t="shared" si="2"/>
-        <v>K0103009801663,SASTH46@,NAJWA INDAH LESTARI,(XII MPLB 1),K0103009801663@gmail.com,XII MPLB 1</v>
+        <v>K0103009801663,SASTH46,NAJWA INDAH LESTARI,(XII MPLB 1),K0103009801663@gmail.com,XII MPLB 1</v>
       </c>
     </row>
     <row r="168" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A168" s="1" t="s">
         <v>425</v>
       </c>
-      <c r="B168" s="2" t="s">
+      <c r="B168" t="s">
         <v>760</v>
       </c>
       <c r="C168" s="1" t="s">
@@ -7210,14 +7215,14 @@
       </c>
       <c r="G168" t="str">
         <f t="shared" si="2"/>
-        <v>K0103009801672,SASTH46@,NATASYA ALAWIYAH,(XII MPLB 1),K0103009801672@gmail.com,XII MPLB 1</v>
+        <v>K0103009801672,SASTH46,NATASYA ALAWIYAH,(XII MPLB 1),K0103009801672@gmail.com,XII MPLB 1</v>
       </c>
     </row>
     <row r="169" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A169" s="1" t="s">
         <v>426</v>
       </c>
-      <c r="B169" s="2" t="s">
+      <c r="B169" t="s">
         <v>760</v>
       </c>
       <c r="C169" s="1" t="s">
@@ -7234,14 +7239,14 @@
       </c>
       <c r="G169" t="str">
         <f t="shared" si="2"/>
-        <v>K0103009801689,SASTH46@,NURUL ZHAHRANI,(XII MPLB 1),K0103009801689@gmail.com,XII MPLB 1</v>
+        <v>K0103009801689,SASTH46,NURUL ZHAHRANI,(XII MPLB 1),K0103009801689@gmail.com,XII MPLB 1</v>
       </c>
     </row>
     <row r="170" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A170" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="B170" s="2" t="s">
+      <c r="B170" t="s">
         <v>760</v>
       </c>
       <c r="C170" s="1" t="s">
@@ -7258,14 +7263,14 @@
       </c>
       <c r="G170" t="str">
         <f t="shared" si="2"/>
-        <v>K0103009801698,SASTH46@,REVALIA RAHMAWATI,(XII MPLB 1),K0103009801698@gmail.com,XII MPLB 1</v>
+        <v>K0103009801698,SASTH46,REVALIA RAHMAWATI,(XII MPLB 1),K0103009801698@gmail.com,XII MPLB 1</v>
       </c>
     </row>
     <row r="171" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A171" s="1" t="s">
         <v>428</v>
       </c>
-      <c r="B171" s="2" t="s">
+      <c r="B171" t="s">
         <v>760</v>
       </c>
       <c r="C171" s="1" t="s">
@@ -7282,14 +7287,14 @@
       </c>
       <c r="G171" t="str">
         <f t="shared" si="2"/>
-        <v>K0103009801707,SASTH46@,RISTY INDRIANI PUTRI,(XII MPLB 1),K0103009801707@gmail.com,XII MPLB 1</v>
+        <v>K0103009801707,SASTH46,RISTY INDRIANI PUTRI,(XII MPLB 1),K0103009801707@gmail.com,XII MPLB 1</v>
       </c>
     </row>
     <row r="172" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A172" s="1" t="s">
         <v>429</v>
       </c>
-      <c r="B172" s="2" t="s">
+      <c r="B172" t="s">
         <v>760</v>
       </c>
       <c r="C172" s="1" t="s">
@@ -7306,14 +7311,14 @@
       </c>
       <c r="G172" t="str">
         <f t="shared" si="2"/>
-        <v>K0103009801716,SASTH46@,SILVIANA NUGRAHA,(XII MPLB 1),K0103009801716@gmail.com,XII MPLB 1</v>
+        <v>K0103009801716,SASTH46,SILVIANA NUGRAHA,(XII MPLB 1),K0103009801716@gmail.com,XII MPLB 1</v>
       </c>
     </row>
     <row r="173" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A173" s="1" t="s">
         <v>430</v>
       </c>
-      <c r="B173" s="2" t="s">
+      <c r="B173" t="s">
         <v>760</v>
       </c>
       <c r="C173" s="1" t="s">
@@ -7330,14 +7335,14 @@
       </c>
       <c r="G173" t="str">
         <f t="shared" si="2"/>
-        <v>K0103009801725,SASTH46@,SILVIE,(XII MPLB 1),K0103009801725@gmail.com,XII MPLB 1</v>
+        <v>K0103009801725,SASTH46,SILVIE,(XII MPLB 1),K0103009801725@gmail.com,XII MPLB 1</v>
       </c>
     </row>
     <row r="174" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A174" s="1" t="s">
         <v>431</v>
       </c>
-      <c r="B174" s="2" t="s">
+      <c r="B174" t="s">
         <v>760</v>
       </c>
       <c r="C174" s="1" t="s">
@@ -7354,14 +7359,14 @@
       </c>
       <c r="G174" t="str">
         <f t="shared" si="2"/>
-        <v>K0103009801734,SASTH46@,SITI TWANTI,(XII MPLB 1),K0103009801734@gmail.com,XII MPLB 1</v>
+        <v>K0103009801734,SASTH46,SITI TWANTI,(XII MPLB 1),K0103009801734@gmail.com,XII MPLB 1</v>
       </c>
     </row>
     <row r="175" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A175" s="1" t="s">
         <v>432</v>
       </c>
-      <c r="B175" s="2" t="s">
+      <c r="B175" t="s">
         <v>760</v>
       </c>
       <c r="C175" s="1" t="s">
@@ -7378,14 +7383,14 @@
       </c>
       <c r="G175" t="str">
         <f t="shared" si="2"/>
-        <v>K0103009801743,SASTH46@,SOFHIANA PUTRI SUTRISNO,(XII MPLB 1),K0103009801743@gmail.com,XII MPLB 1</v>
+        <v>K0103009801743,SASTH46,SOFHIANA PUTRI SUTRISNO,(XII MPLB 1),K0103009801743@gmail.com,XII MPLB 1</v>
       </c>
     </row>
     <row r="176" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A176" s="1" t="s">
         <v>433</v>
       </c>
-      <c r="B176" s="2" t="s">
+      <c r="B176" t="s">
         <v>760</v>
       </c>
       <c r="C176" s="1" t="s">
@@ -7402,14 +7407,14 @@
       </c>
       <c r="G176" t="str">
         <f t="shared" si="2"/>
-        <v>K0103009801752,SASTH46@,VIVIAN CORNELIA SETIAWAN,(XII MPLB 1),K0103009801752@gmail.com,XII MPLB 1</v>
+        <v>K0103009801752,SASTH46,VIVIAN CORNELIA SETIAWAN,(XII MPLB 1),K0103009801752@gmail.com,XII MPLB 1</v>
       </c>
     </row>
     <row r="177" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A177" s="1" t="s">
         <v>434</v>
       </c>
-      <c r="B177" s="2" t="s">
+      <c r="B177" t="s">
         <v>760</v>
       </c>
       <c r="C177" s="1" t="s">
@@ -7426,14 +7431,14 @@
       </c>
       <c r="G177" t="str">
         <f t="shared" si="2"/>
-        <v>K0103009801769,SASTH46@,ADELIA ZAHRA KHIRANA,(XII MPLB 2),K0103009801769@gmail.com,XII MPLB 2</v>
+        <v>K0103009801769,SASTH46,ADELIA ZAHRA KHIRANA,(XII MPLB 2),K0103009801769@gmail.com,XII MPLB 2</v>
       </c>
     </row>
     <row r="178" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A178" s="1" t="s">
         <v>435</v>
       </c>
-      <c r="B178" s="2" t="s">
+      <c r="B178" t="s">
         <v>760</v>
       </c>
       <c r="C178" s="1" t="s">
@@ -7450,14 +7455,14 @@
       </c>
       <c r="G178" t="str">
         <f t="shared" si="2"/>
-        <v>K0103009801778,SASTH46@,AMANDA NURMALA,(XII MPLB 2),K0103009801778@gmail.com,XII MPLB 2</v>
+        <v>K0103009801778,SASTH46,AMANDA NURMALA,(XII MPLB 2),K0103009801778@gmail.com,XII MPLB 2</v>
       </c>
     </row>
     <row r="179" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A179" s="1" t="s">
         <v>436</v>
       </c>
-      <c r="B179" s="2" t="s">
+      <c r="B179" t="s">
         <v>760</v>
       </c>
       <c r="C179" s="1" t="s">
@@ -7474,14 +7479,14 @@
       </c>
       <c r="G179" t="str">
         <f t="shared" si="2"/>
-        <v>K0103009801787,SASTH46@,ANIS SYAHIIDAH MEILANI,(XII MPLB 2),K0103009801787@gmail.com,XII MPLB 2</v>
+        <v>K0103009801787,SASTH46,ANIS SYAHIIDAH MEILANI,(XII MPLB 2),K0103009801787@gmail.com,XII MPLB 2</v>
       </c>
     </row>
     <row r="180" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A180" s="1" t="s">
         <v>437</v>
       </c>
-      <c r="B180" s="2" t="s">
+      <c r="B180" t="s">
         <v>760</v>
       </c>
       <c r="C180" s="1" t="s">
@@ -7498,14 +7503,14 @@
       </c>
       <c r="G180" t="str">
         <f t="shared" si="2"/>
-        <v>K0103009801796,SASTH46@,ANISSA,(XII MPLB 2),K0103009801796@gmail.com,XII MPLB 2</v>
+        <v>K0103009801796,SASTH46,ANISSA,(XII MPLB 2),K0103009801796@gmail.com,XII MPLB 2</v>
       </c>
     </row>
     <row r="181" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A181" s="1" t="s">
         <v>438</v>
       </c>
-      <c r="B181" s="2" t="s">
+      <c r="B181" t="s">
         <v>760</v>
       </c>
       <c r="C181" s="1" t="s">
@@ -7522,14 +7527,14 @@
       </c>
       <c r="G181" t="str">
         <f t="shared" si="2"/>
-        <v>K0103009801805,SASTH46@,ASHA SHARA APRIANA,(XII MPLB 2),K0103009801805@gmail.com,XII MPLB 2</v>
+        <v>K0103009801805,SASTH46,ASHA SHARA APRIANA,(XII MPLB 2),K0103009801805@gmail.com,XII MPLB 2</v>
       </c>
     </row>
     <row r="182" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A182" s="1" t="s">
         <v>439</v>
       </c>
-      <c r="B182" s="2" t="s">
+      <c r="B182" t="s">
         <v>760</v>
       </c>
       <c r="C182" s="1" t="s">
@@ -7546,14 +7551,14 @@
       </c>
       <c r="G182" t="str">
         <f t="shared" si="2"/>
-        <v>K0103009801814,SASTH46@,AZ ZAHRA ZIDNI NAYSABILLA,(XII MPLB 2),K0103009801814@gmail.com,XII MPLB 2</v>
+        <v>K0103009801814,SASTH46,AZ ZAHRA ZIDNI NAYSABILLA,(XII MPLB 2),K0103009801814@gmail.com,XII MPLB 2</v>
       </c>
     </row>
     <row r="183" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A183" s="1" t="s">
         <v>440</v>
       </c>
-      <c r="B183" s="2" t="s">
+      <c r="B183" t="s">
         <v>760</v>
       </c>
       <c r="C183" s="1" t="s">
@@ -7570,14 +7575,14 @@
       </c>
       <c r="G183" t="str">
         <f t="shared" si="2"/>
-        <v>K0103009801823,SASTH46@,DEA RAHMA ALYA,(XII MPLB 2),K0103009801823@gmail.com,XII MPLB 2</v>
+        <v>K0103009801823,SASTH46,DEA RAHMA ALYA,(XII MPLB 2),K0103009801823@gmail.com,XII MPLB 2</v>
       </c>
     </row>
     <row r="184" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A184" s="1" t="s">
         <v>441</v>
       </c>
-      <c r="B184" s="2" t="s">
+      <c r="B184" t="s">
         <v>760</v>
       </c>
       <c r="C184" s="1" t="s">
@@ -7594,14 +7599,14 @@
       </c>
       <c r="G184" t="str">
         <f t="shared" si="2"/>
-        <v>K0103009801832,SASTH46@,DHEA RAHMAWATI,(XII MPLB 2),K0103009801832@gmail.com,XII MPLB 2</v>
+        <v>K0103009801832,SASTH46,DHEA RAHMAWATI,(XII MPLB 2),K0103009801832@gmail.com,XII MPLB 2</v>
       </c>
     </row>
     <row r="185" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A185" s="1" t="s">
         <v>442</v>
       </c>
-      <c r="B185" s="2" t="s">
+      <c r="B185" t="s">
         <v>760</v>
       </c>
       <c r="C185" s="1" t="s">
@@ -7618,14 +7623,14 @@
       </c>
       <c r="G185" t="str">
         <f t="shared" si="2"/>
-        <v>K0103009801849,SASTH46@,FIKA DAVILA,(XII MPLB 2),K0103009801849@gmail.com,XII MPLB 2</v>
+        <v>K0103009801849,SASTH46,FIKA DAVILA,(XII MPLB 2),K0103009801849@gmail.com,XII MPLB 2</v>
       </c>
     </row>
     <row r="186" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A186" s="1" t="s">
         <v>443</v>
       </c>
-      <c r="B186" s="2" t="s">
+      <c r="B186" t="s">
         <v>760</v>
       </c>
       <c r="C186" s="1" t="s">
@@ -7642,14 +7647,14 @@
       </c>
       <c r="G186" t="str">
         <f t="shared" si="2"/>
-        <v>K0103009801858,SASTH46@,FLORA CINDY AULIA,(XII MPLB 2),K0103009801858@gmail.com,XII MPLB 2</v>
+        <v>K0103009801858,SASTH46,FLORA CINDY AULIA,(XII MPLB 2),K0103009801858@gmail.com,XII MPLB 2</v>
       </c>
     </row>
     <row r="187" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A187" s="1" t="s">
         <v>444</v>
       </c>
-      <c r="B187" s="2" t="s">
+      <c r="B187" t="s">
         <v>760</v>
       </c>
       <c r="C187" s="1" t="s">
@@ -7666,14 +7671,14 @@
       </c>
       <c r="G187" t="str">
         <f t="shared" si="2"/>
-        <v>K0103009801867,SASTH46@,IRMA SEPTIANI IRWANSYAH,(XII MPLB 2),K0103009801867@gmail.com,XII MPLB 2</v>
+        <v>K0103009801867,SASTH46,IRMA SEPTIANI IRWANSYAH,(XII MPLB 2),K0103009801867@gmail.com,XII MPLB 2</v>
       </c>
     </row>
     <row r="188" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A188" s="1" t="s">
         <v>445</v>
       </c>
-      <c r="B188" s="2" t="s">
+      <c r="B188" t="s">
         <v>760</v>
       </c>
       <c r="C188" s="1" t="s">
@@ -7690,14 +7695,14 @@
       </c>
       <c r="G188" t="str">
         <f t="shared" si="2"/>
-        <v>K0103009801876,SASTH46@,KHUSNUL KHOTIMATUL ZAHRA,(XII MPLB 2),K0103009801876@gmail.com,XII MPLB 2</v>
+        <v>K0103009801876,SASTH46,KHUSNUL KHOTIMATUL ZAHRA,(XII MPLB 2),K0103009801876@gmail.com,XII MPLB 2</v>
       </c>
     </row>
     <row r="189" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A189" s="1" t="s">
         <v>446</v>
       </c>
-      <c r="B189" s="2" t="s">
+      <c r="B189" t="s">
         <v>760</v>
       </c>
       <c r="C189" s="1" t="s">
@@ -7714,14 +7719,14 @@
       </c>
       <c r="G189" t="str">
         <f t="shared" si="2"/>
-        <v>K0103009801885,SASTH46@,NABILA PUTRI SETIAWAN,(XII MPLB 2),K0103009801885@gmail.com,XII MPLB 2</v>
+        <v>K0103009801885,SASTH46,NABILA PUTRI SETIAWAN,(XII MPLB 2),K0103009801885@gmail.com,XII MPLB 2</v>
       </c>
     </row>
     <row r="190" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A190" s="1" t="s">
         <v>447</v>
       </c>
-      <c r="B190" s="2" t="s">
+      <c r="B190" t="s">
         <v>760</v>
       </c>
       <c r="C190" s="1" t="s">
@@ -7738,14 +7743,14 @@
       </c>
       <c r="G190" t="str">
         <f t="shared" si="2"/>
-        <v>K0103009801894,SASTH46@,NABILA SEPTIYANA DEWI,(XII MPLB 2),K0103009801894@gmail.com,XII MPLB 2</v>
+        <v>K0103009801894,SASTH46,NABILA SEPTIYANA DEWI,(XII MPLB 2),K0103009801894@gmail.com,XII MPLB 2</v>
       </c>
     </row>
     <row r="191" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A191" s="1" t="s">
         <v>448</v>
       </c>
-      <c r="B191" s="2" t="s">
+      <c r="B191" t="s">
         <v>760</v>
       </c>
       <c r="C191" s="1" t="s">
@@ -7762,14 +7767,14 @@
       </c>
       <c r="G191" t="str">
         <f t="shared" si="2"/>
-        <v>K0103009801903,SASTH46@,NABYLA,(XII MPLB 2),K0103009801903@gmail.com,XII MPLB 2</v>
+        <v>K0103009801903,SASTH46,NABYLA,(XII MPLB 2),K0103009801903@gmail.com,XII MPLB 2</v>
       </c>
     </row>
     <row r="192" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A192" s="1" t="s">
         <v>449</v>
       </c>
-      <c r="B192" s="2" t="s">
+      <c r="B192" t="s">
         <v>760</v>
       </c>
       <c r="C192" s="1" t="s">
@@ -7786,14 +7791,14 @@
       </c>
       <c r="G192" t="str">
         <f t="shared" si="2"/>
-        <v>K0103009801912,SASTH46@,NANDITA PUTRI RAMADHANI,(XII MPLB 2),K0103009801912@gmail.com,XII MPLB 2</v>
+        <v>K0103009801912,SASTH46,NANDITA PUTRI RAMADHANI,(XII MPLB 2),K0103009801912@gmail.com,XII MPLB 2</v>
       </c>
     </row>
     <row r="193" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A193" s="1" t="s">
         <v>450</v>
       </c>
-      <c r="B193" s="2" t="s">
+      <c r="B193" t="s">
         <v>760</v>
       </c>
       <c r="C193" s="1" t="s">
@@ -7810,14 +7815,14 @@
       </c>
       <c r="G193" t="str">
         <f t="shared" si="2"/>
-        <v>K0103009801929,SASTH46@,NEZA CHARLITA,(XII MPLB 2),K0103009801929@gmail.com,XII MPLB 2</v>
+        <v>K0103009801929,SASTH46,NEZA CHARLITA,(XII MPLB 2),K0103009801929@gmail.com,XII MPLB 2</v>
       </c>
     </row>
     <row r="194" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A194" s="1" t="s">
         <v>451</v>
       </c>
-      <c r="B194" s="2" t="s">
+      <c r="B194" t="s">
         <v>760</v>
       </c>
       <c r="C194" s="1" t="s">
@@ -7834,14 +7839,14 @@
       </c>
       <c r="G194" t="str">
         <f t="shared" ref="G194:G247" si="3">CONCATENATE(A194,",",B194,",",C194,",",D194,",",E194,",",F194)</f>
-        <v>K0103009801938,SASTH46@,NIMAS NUR YAUMI,(XII MPLB 2),K0103009801938@gmail.com,XII MPLB 2</v>
+        <v>K0103009801938,SASTH46,NIMAS NUR YAUMI,(XII MPLB 2),K0103009801938@gmail.com,XII MPLB 2</v>
       </c>
     </row>
     <row r="195" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A195" s="1" t="s">
         <v>452</v>
       </c>
-      <c r="B195" s="2" t="s">
+      <c r="B195" t="s">
         <v>760</v>
       </c>
       <c r="C195" s="1" t="s">
@@ -7858,14 +7863,14 @@
       </c>
       <c r="G195" t="str">
         <f t="shared" si="3"/>
-        <v>K0103009801947,SASTH46@,NIRMALASARI,(XII MPLB 2),K0103009801947@gmail.com,XII MPLB 2</v>
+        <v>K0103009801947,SASTH46,NIRMALASARI,(XII MPLB 2),K0103009801947@gmail.com,XII MPLB 2</v>
       </c>
     </row>
     <row r="196" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A196" s="1" t="s">
         <v>453</v>
       </c>
-      <c r="B196" s="2" t="s">
+      <c r="B196" t="s">
         <v>760</v>
       </c>
       <c r="C196" s="1" t="s">
@@ -7882,14 +7887,14 @@
       </c>
       <c r="G196" t="str">
         <f t="shared" si="3"/>
-        <v>K0103009801956,SASTH46@,NOVIA AMANDA,(XII MPLB 2),K0103009801956@gmail.com,XII MPLB 2</v>
+        <v>K0103009801956,SASTH46,NOVIA AMANDA,(XII MPLB 2),K0103009801956@gmail.com,XII MPLB 2</v>
       </c>
     </row>
     <row r="197" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A197" s="1" t="s">
         <v>454</v>
       </c>
-      <c r="B197" s="2" t="s">
+      <c r="B197" t="s">
         <v>760</v>
       </c>
       <c r="C197" s="1" t="s">
@@ -7906,14 +7911,14 @@
       </c>
       <c r="G197" t="str">
         <f t="shared" si="3"/>
-        <v>K0103009801965,SASTH46@,NURHIKMAH,(XII MPLB 2),K0103009801965@gmail.com,XII MPLB 2</v>
+        <v>K0103009801965,SASTH46,NURHIKMAH,(XII MPLB 2),K0103009801965@gmail.com,XII MPLB 2</v>
       </c>
     </row>
     <row r="198" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A198" s="1" t="s">
         <v>455</v>
       </c>
-      <c r="B198" s="2" t="s">
+      <c r="B198" t="s">
         <v>760</v>
       </c>
       <c r="C198" s="1" t="s">
@@ -7930,14 +7935,14 @@
       </c>
       <c r="G198" t="str">
         <f t="shared" si="3"/>
-        <v>K0103009801974,SASTH46@,PUTRI AYU WULANDARI,(XII MPLB 2),K0103009801974@gmail.com,XII MPLB 2</v>
+        <v>K0103009801974,SASTH46,PUTRI AYU WULANDARI,(XII MPLB 2),K0103009801974@gmail.com,XII MPLB 2</v>
       </c>
     </row>
     <row r="199" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A199" s="1" t="s">
         <v>456</v>
       </c>
-      <c r="B199" s="2" t="s">
+      <c r="B199" t="s">
         <v>760</v>
       </c>
       <c r="C199" s="1" t="s">
@@ -7954,14 +7959,14 @@
       </c>
       <c r="G199" t="str">
         <f t="shared" si="3"/>
-        <v>K0103009801983,SASTH46@,RATNA DILAH,(XII MPLB 2),K0103009801983@gmail.com,XII MPLB 2</v>
+        <v>K0103009801983,SASTH46,RATNA DILAH,(XII MPLB 2),K0103009801983@gmail.com,XII MPLB 2</v>
       </c>
     </row>
     <row r="200" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A200" s="1" t="s">
         <v>457</v>
       </c>
-      <c r="B200" s="2" t="s">
+      <c r="B200" t="s">
         <v>760</v>
       </c>
       <c r="C200" s="1" t="s">
@@ -7978,14 +7983,14 @@
       </c>
       <c r="G200" t="str">
         <f t="shared" si="3"/>
-        <v>K0103009801992,SASTH46@,RINI NURBAITI,(XII MPLB 2),K0103009801992@gmail.com,XII MPLB 2</v>
+        <v>K0103009801992,SASTH46,RINI NURBAITI,(XII MPLB 2),K0103009801992@gmail.com,XII MPLB 2</v>
       </c>
     </row>
     <row r="201" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A201" s="1" t="s">
         <v>458</v>
       </c>
-      <c r="B201" s="2" t="s">
+      <c r="B201" t="s">
         <v>760</v>
       </c>
       <c r="C201" s="1" t="s">
@@ -8002,14 +8007,14 @@
       </c>
       <c r="G201" t="str">
         <f t="shared" si="3"/>
-        <v>K0103009802009,SASTH46@,RIYANTI WAFIQ AZIZAH,(XII MPLB 2),K0103009802009@gmail.com,XII MPLB 2</v>
+        <v>K0103009802009,SASTH46,RIYANTI WAFIQ AZIZAH,(XII MPLB 2),K0103009802009@gmail.com,XII MPLB 2</v>
       </c>
     </row>
     <row r="202" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A202" s="1" t="s">
         <v>459</v>
       </c>
-      <c r="B202" s="2" t="s">
+      <c r="B202" t="s">
         <v>760</v>
       </c>
       <c r="C202" s="1" t="s">
@@ -8026,14 +8031,14 @@
       </c>
       <c r="G202" t="str">
         <f t="shared" si="3"/>
-        <v>K0103009802018,SASTH46@,SALSABILA NURUL FITRI,(XII MPLB 2),K0103009802018@gmail.com,XII MPLB 2</v>
+        <v>K0103009802018,SASTH46,SALSABILA NURUL FITRI,(XII MPLB 2),K0103009802018@gmail.com,XII MPLB 2</v>
       </c>
     </row>
     <row r="203" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A203" s="1" t="s">
         <v>460</v>
       </c>
-      <c r="B203" s="2" t="s">
+      <c r="B203" t="s">
         <v>760</v>
       </c>
       <c r="C203" s="1" t="s">
@@ -8050,14 +8055,14 @@
       </c>
       <c r="G203" t="str">
         <f t="shared" si="3"/>
-        <v>K0103009802027,SASTH46@,SITI MUTIARA WARDAH,(XII MPLB 2),K0103009802027@gmail.com,XII MPLB 2</v>
+        <v>K0103009802027,SASTH46,SITI MUTIARA WARDAH,(XII MPLB 2),K0103009802027@gmail.com,XII MPLB 2</v>
       </c>
     </row>
     <row r="204" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A204" s="1" t="s">
         <v>461</v>
       </c>
-      <c r="B204" s="2" t="s">
+      <c r="B204" t="s">
         <v>760</v>
       </c>
       <c r="C204" s="1" t="s">
@@ -8074,14 +8079,14 @@
       </c>
       <c r="G204" t="str">
         <f t="shared" si="3"/>
-        <v>K0103009802036,SASTH46@,SYAIRA RANI ASMARI PUTRI,(XII MPLB 2),K0103009802036@gmail.com,XII MPLB 2</v>
+        <v>K0103009802036,SASTH46,SYAIRA RANI ASMARI PUTRI,(XII MPLB 2),K0103009802036@gmail.com,XII MPLB 2</v>
       </c>
     </row>
     <row r="205" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A205" s="1" t="s">
         <v>462</v>
       </c>
-      <c r="B205" s="2" t="s">
+      <c r="B205" t="s">
         <v>760</v>
       </c>
       <c r="C205" s="1" t="s">
@@ -8098,14 +8103,14 @@
       </c>
       <c r="G205" t="str">
         <f t="shared" si="3"/>
-        <v>K0103009802045,SASTH46@,TASYA MUT'ALIFAH,(XII MPLB 2),K0103009802045@gmail.com,XII MPLB 2</v>
+        <v>K0103009802045,SASTH46,TASYA MUT'ALIFAH,(XII MPLB 2),K0103009802045@gmail.com,XII MPLB 2</v>
       </c>
     </row>
     <row r="206" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A206" s="1" t="s">
         <v>463</v>
       </c>
-      <c r="B206" s="2" t="s">
+      <c r="B206" t="s">
         <v>760</v>
       </c>
       <c r="C206" s="1" t="s">
@@ -8122,14 +8127,14 @@
       </c>
       <c r="G206" t="str">
         <f t="shared" si="3"/>
-        <v>K0103009802054,SASTH46@,TRIA KARTINI WAHYUDI,(XII MPLB 2),K0103009802054@gmail.com,XII MPLB 2</v>
+        <v>K0103009802054,SASTH46,TRIA KARTINI WAHYUDI,(XII MPLB 2),K0103009802054@gmail.com,XII MPLB 2</v>
       </c>
     </row>
     <row r="207" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A207" s="1" t="s">
         <v>464</v>
       </c>
-      <c r="B207" s="2" t="s">
+      <c r="B207" t="s">
         <v>760</v>
       </c>
       <c r="C207" s="1" t="s">
@@ -8146,14 +8151,14 @@
       </c>
       <c r="G207" t="str">
         <f t="shared" si="3"/>
-        <v>K0103009802063,SASTH46@,WINDA AULIA,(XII MPLB 2),K0103009802063@gmail.com,XII MPLB 2</v>
+        <v>K0103009802063,SASTH46,WINDA AULIA,(XII MPLB 2),K0103009802063@gmail.com,XII MPLB 2</v>
       </c>
     </row>
     <row r="208" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A208" s="1" t="s">
         <v>465</v>
       </c>
-      <c r="B208" s="2" t="s">
+      <c r="B208" t="s">
         <v>760</v>
       </c>
       <c r="C208" s="1" t="s">
@@ -8170,14 +8175,14 @@
       </c>
       <c r="G208" t="str">
         <f t="shared" si="3"/>
-        <v>K0103009802072,SASTH46@,WINDA RESTU FALIHA,(XII MPLB 2),K0103009802072@gmail.com,XII MPLB 2</v>
+        <v>K0103009802072,SASTH46,WINDA RESTU FALIHA,(XII MPLB 2),K0103009802072@gmail.com,XII MPLB 2</v>
       </c>
     </row>
     <row r="209" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A209" s="1" t="s">
         <v>466</v>
       </c>
-      <c r="B209" s="2" t="s">
+      <c r="B209" t="s">
         <v>760</v>
       </c>
       <c r="C209" s="1" t="s">
@@ -8194,14 +8199,14 @@
       </c>
       <c r="G209" t="str">
         <f t="shared" si="3"/>
-        <v>K0103009802089,SASTH46@,AKBAR SADEWA,(XII PM),K0103009802089@gmail.com,XII PM</v>
+        <v>K0103009802089,SASTH46,AKBAR SADEWA,(XII PM),K0103009802089@gmail.com,XII PM</v>
       </c>
     </row>
     <row r="210" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A210" s="1" t="s">
         <v>467</v>
       </c>
-      <c r="B210" s="2" t="s">
+      <c r="B210" t="s">
         <v>760</v>
       </c>
       <c r="C210" s="1" t="s">
@@ -8218,14 +8223,14 @@
       </c>
       <c r="G210" t="str">
         <f t="shared" si="3"/>
-        <v>K0103009802098,SASTH46@,ANDHIKA DIAN SAPUTRA,(XII PM),K0103009802098@gmail.com,XII PM</v>
+        <v>K0103009802098,SASTH46,ANDHIKA DIAN SAPUTRA,(XII PM),K0103009802098@gmail.com,XII PM</v>
       </c>
     </row>
     <row r="211" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A211" s="1" t="s">
         <v>468</v>
       </c>
-      <c r="B211" s="2" t="s">
+      <c r="B211" t="s">
         <v>760</v>
       </c>
       <c r="C211" s="1" t="s">
@@ -8242,14 +8247,14 @@
       </c>
       <c r="G211" t="str">
         <f t="shared" si="3"/>
-        <v>K0103009802107,SASTH46@,ANDRE YULIANTO,(XII PM),K0103009802107@gmail.com,XII PM</v>
+        <v>K0103009802107,SASTH46,ANDRE YULIANTO,(XII PM),K0103009802107@gmail.com,XII PM</v>
       </c>
     </row>
     <row r="212" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A212" s="1" t="s">
         <v>469</v>
       </c>
-      <c r="B212" s="2" t="s">
+      <c r="B212" t="s">
         <v>760</v>
       </c>
       <c r="C212" s="1" t="s">
@@ -8266,14 +8271,14 @@
       </c>
       <c r="G212" t="str">
         <f t="shared" si="3"/>
-        <v>K0103009802116,SASTH46@,ARDIONA ATTA SAPUTRA,(XII PM),K0103009802116@gmail.com,XII PM</v>
+        <v>K0103009802116,SASTH46,ARDIONA ATTA SAPUTRA,(XII PM),K0103009802116@gmail.com,XII PM</v>
       </c>
     </row>
     <row r="213" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A213" s="1" t="s">
         <v>470</v>
       </c>
-      <c r="B213" s="2" t="s">
+      <c r="B213" t="s">
         <v>760</v>
       </c>
       <c r="C213" s="1" t="s">
@@ -8290,14 +8295,14 @@
       </c>
       <c r="G213" t="str">
         <f t="shared" si="3"/>
-        <v>K0103009802125,SASTH46@,BAHRUDIN SIROTH,(XII PM),K0103009802125@gmail.com,XII PM</v>
+        <v>K0103009802125,SASTH46,BAHRUDIN SIROTH,(XII PM),K0103009802125@gmail.com,XII PM</v>
       </c>
     </row>
     <row r="214" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A214" s="1" t="s">
         <v>471</v>
       </c>
-      <c r="B214" s="2" t="s">
+      <c r="B214" t="s">
         <v>760</v>
       </c>
       <c r="C214" s="1" t="s">
@@ -8314,14 +8319,14 @@
       </c>
       <c r="G214" t="str">
         <f t="shared" si="3"/>
-        <v>K0103009802134,SASTH46@,BRILLIANT MUHAMMAD PRANAYA,(XII PM),K0103009802134@gmail.com,XII PM</v>
+        <v>K0103009802134,SASTH46,BRILLIANT MUHAMMAD PRANAYA,(XII PM),K0103009802134@gmail.com,XII PM</v>
       </c>
     </row>
     <row r="215" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A215" s="1" t="s">
         <v>472</v>
       </c>
-      <c r="B215" s="2" t="s">
+      <c r="B215" t="s">
         <v>760</v>
       </c>
       <c r="C215" s="1" t="s">
@@ -8338,14 +8343,14 @@
       </c>
       <c r="G215" t="str">
         <f t="shared" si="3"/>
-        <v>K0103009802143,SASTH46@,CHINDY WULAN SARI,(XII PM),K0103009802143@gmail.com,XII PM</v>
+        <v>K0103009802143,SASTH46,CHINDY WULAN SARI,(XII PM),K0103009802143@gmail.com,XII PM</v>
       </c>
     </row>
     <row r="216" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A216" s="1" t="s">
         <v>473</v>
       </c>
-      <c r="B216" s="2" t="s">
+      <c r="B216" t="s">
         <v>760</v>
       </c>
       <c r="C216" s="1" t="s">
@@ -8362,14 +8367,14 @@
       </c>
       <c r="G216" t="str">
         <f t="shared" si="3"/>
-        <v>K0103009802152,SASTH46@,DAYDAEL RAHMAT PRIHARTONO,(XII PM),K0103009802152@gmail.com,XII PM</v>
+        <v>K0103009802152,SASTH46,DAYDAEL RAHMAT PRIHARTONO,(XII PM),K0103009802152@gmail.com,XII PM</v>
       </c>
     </row>
     <row r="217" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A217" s="1" t="s">
         <v>474</v>
       </c>
-      <c r="B217" s="2" t="s">
+      <c r="B217" t="s">
         <v>760</v>
       </c>
       <c r="C217" s="1" t="s">
@@ -8386,14 +8391,14 @@
       </c>
       <c r="G217" t="str">
         <f t="shared" si="3"/>
-        <v>K0103009802169,SASTH46@,DEVINNA CHRISTIANAH,(XII PM),K0103009802169@gmail.com,XII PM</v>
+        <v>K0103009802169,SASTH46,DEVINNA CHRISTIANAH,(XII PM),K0103009802169@gmail.com,XII PM</v>
       </c>
     </row>
     <row r="218" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A218" s="1" t="s">
         <v>475</v>
       </c>
-      <c r="B218" s="2" t="s">
+      <c r="B218" t="s">
         <v>760</v>
       </c>
       <c r="C218" s="1" t="s">
@@ -8410,14 +8415,14 @@
       </c>
       <c r="G218" t="str">
         <f t="shared" si="3"/>
-        <v>K0103009802178,SASTH46@,DIANA FEBRIASTUTI,(XII PM),K0103009802178@gmail.com,XII PM</v>
+        <v>K0103009802178,SASTH46,DIANA FEBRIASTUTI,(XII PM),K0103009802178@gmail.com,XII PM</v>
       </c>
     </row>
     <row r="219" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A219" s="1" t="s">
         <v>476</v>
       </c>
-      <c r="B219" s="2" t="s">
+      <c r="B219" t="s">
         <v>760</v>
       </c>
       <c r="C219" s="1" t="s">
@@ -8434,14 +8439,14 @@
       </c>
       <c r="G219" t="str">
         <f t="shared" si="3"/>
-        <v>K0103009802187,SASTH46@,DIKI MUZALFA,(XII PM),K0103009802187@gmail.com,XII PM</v>
+        <v>K0103009802187,SASTH46,DIKI MUZALFA,(XII PM),K0103009802187@gmail.com,XII PM</v>
       </c>
     </row>
     <row r="220" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A220" s="1" t="s">
         <v>477</v>
       </c>
-      <c r="B220" s="2" t="s">
+      <c r="B220" t="s">
         <v>760</v>
       </c>
       <c r="C220" s="1" t="s">
@@ -8458,14 +8463,14 @@
       </c>
       <c r="G220" t="str">
         <f t="shared" si="3"/>
-        <v>K0103009802196,SASTH46@,DINI AULIA,(XII PM),K0103009802196@gmail.com,XII PM</v>
+        <v>K0103009802196,SASTH46,DINI AULIA,(XII PM),K0103009802196@gmail.com,XII PM</v>
       </c>
     </row>
     <row r="221" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A221" s="1" t="s">
         <v>478</v>
       </c>
-      <c r="B221" s="2" t="s">
+      <c r="B221" t="s">
         <v>760</v>
       </c>
       <c r="C221" s="1" t="s">
@@ -8482,14 +8487,14 @@
       </c>
       <c r="G221" t="str">
         <f t="shared" si="3"/>
-        <v>K0103009802205,SASTH46@,FAKHRIY PUTRA MAULANA,(XII PM),K0103009802205@gmail.com,XII PM</v>
+        <v>K0103009802205,SASTH46,FAKHRIY PUTRA MAULANA,(XII PM),K0103009802205@gmail.com,XII PM</v>
       </c>
     </row>
     <row r="222" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A222" s="1" t="s">
         <v>479</v>
       </c>
-      <c r="B222" s="2" t="s">
+      <c r="B222" t="s">
         <v>760</v>
       </c>
       <c r="C222" s="1" t="s">
@@ -8506,14 +8511,14 @@
       </c>
       <c r="G222" t="str">
         <f t="shared" si="3"/>
-        <v>K0103009802214,SASTH46@,FIONA FASTAG FARA,(XII PM),K0103009802214@gmail.com,XII PM</v>
+        <v>K0103009802214,SASTH46,FIONA FASTAG FARA,(XII PM),K0103009802214@gmail.com,XII PM</v>
       </c>
     </row>
     <row r="223" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A223" s="1" t="s">
         <v>480</v>
       </c>
-      <c r="B223" s="2" t="s">
+      <c r="B223" t="s">
         <v>760</v>
       </c>
       <c r="C223" s="1" t="s">
@@ -8530,14 +8535,14 @@
       </c>
       <c r="G223" t="str">
         <f t="shared" si="3"/>
-        <v>K0103009802223,SASTH46@,GURUH PRIYANDONO,(XII PM),K0103009802223@gmail.com,XII PM</v>
+        <v>K0103009802223,SASTH46,GURUH PRIYANDONO,(XII PM),K0103009802223@gmail.com,XII PM</v>
       </c>
     </row>
     <row r="224" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A224" s="1" t="s">
         <v>481</v>
       </c>
-      <c r="B224" s="2" t="s">
+      <c r="B224" t="s">
         <v>760</v>
       </c>
       <c r="C224" s="1" t="s">
@@ -8554,14 +8559,14 @@
       </c>
       <c r="G224" t="str">
         <f t="shared" si="3"/>
-        <v>K0103009802232,SASTH46@,HAFISTH IKHSAN MAULANA,(XII PM),K0103009802232@gmail.com,XII PM</v>
+        <v>K0103009802232,SASTH46,HAFISTH IKHSAN MAULANA,(XII PM),K0103009802232@gmail.com,XII PM</v>
       </c>
     </row>
     <row r="225" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A225" s="1" t="s">
         <v>482</v>
       </c>
-      <c r="B225" s="2" t="s">
+      <c r="B225" t="s">
         <v>760</v>
       </c>
       <c r="C225" s="1" t="s">
@@ -8578,14 +8583,14 @@
       </c>
       <c r="G225" t="str">
         <f t="shared" si="3"/>
-        <v>K0103009802249,SASTH46@,JUNEDI,(XII PM),K0103009802249@gmail.com,XII PM</v>
+        <v>K0103009802249,SASTH46,JUNEDI,(XII PM),K0103009802249@gmail.com,XII PM</v>
       </c>
     </row>
     <row r="226" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A226" s="1" t="s">
         <v>483</v>
       </c>
-      <c r="B226" s="2" t="s">
+      <c r="B226" t="s">
         <v>760</v>
       </c>
       <c r="C226" s="1" t="s">
@@ -8602,14 +8607,14 @@
       </c>
       <c r="G226" t="str">
         <f t="shared" si="3"/>
-        <v>K0103009802258,SASTH46@,KEISYA DWI AMELIA,(XII PM),K0103009802258@gmail.com,XII PM</v>
+        <v>K0103009802258,SASTH46,KEISYA DWI AMELIA,(XII PM),K0103009802258@gmail.com,XII PM</v>
       </c>
     </row>
     <row r="227" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A227" s="1" t="s">
         <v>484</v>
       </c>
-      <c r="B227" s="2" t="s">
+      <c r="B227" t="s">
         <v>760</v>
       </c>
       <c r="C227" s="1" t="s">
@@ -8626,14 +8631,14 @@
       </c>
       <c r="G227" t="str">
         <f t="shared" si="3"/>
-        <v>K0103009802267,SASTH46@,MARCELLINO ADI PRATAMA,(XII PM),K0103009802267@gmail.com,XII PM</v>
+        <v>K0103009802267,SASTH46,MARCELLINO ADI PRATAMA,(XII PM),K0103009802267@gmail.com,XII PM</v>
       </c>
     </row>
     <row r="228" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A228" s="1" t="s">
         <v>485</v>
       </c>
-      <c r="B228" s="2" t="s">
+      <c r="B228" t="s">
         <v>760</v>
       </c>
       <c r="C228" s="1" t="s">
@@ -8650,14 +8655,14 @@
       </c>
       <c r="G228" t="str">
         <f t="shared" si="3"/>
-        <v>K0103009802276,SASTH46@,MIFTAHUL SAPUTRA,(XII PM),K0103009802276@gmail.com,XII PM</v>
+        <v>K0103009802276,SASTH46,MIFTAHUL SAPUTRA,(XII PM),K0103009802276@gmail.com,XII PM</v>
       </c>
     </row>
     <row r="229" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A229" s="1" t="s">
         <v>486</v>
       </c>
-      <c r="B229" s="2" t="s">
+      <c r="B229" t="s">
         <v>760</v>
       </c>
       <c r="C229" s="1" t="s">
@@ -8674,14 +8679,14 @@
       </c>
       <c r="G229" t="str">
         <f t="shared" si="3"/>
-        <v>K0103009802285,SASTH46@,MUHAMAD RAKA HADI SANJAYA,(XII PM),K0103009802285@gmail.com,XII PM</v>
+        <v>K0103009802285,SASTH46,MUHAMAD RAKA HADI SANJAYA,(XII PM),K0103009802285@gmail.com,XII PM</v>
       </c>
     </row>
     <row r="230" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A230" s="1" t="s">
         <v>487</v>
       </c>
-      <c r="B230" s="2" t="s">
+      <c r="B230" t="s">
         <v>760</v>
       </c>
       <c r="C230" s="1" t="s">
@@ -8698,14 +8703,14 @@
       </c>
       <c r="G230" t="str">
         <f t="shared" si="3"/>
-        <v>K0103009802294,SASTH46@,MUHAMAD RIANSYAH,(XII PM),K0103009802294@gmail.com,XII PM</v>
+        <v>K0103009802294,SASTH46,MUHAMAD RIANSYAH,(XII PM),K0103009802294@gmail.com,XII PM</v>
       </c>
     </row>
     <row r="231" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A231" s="1" t="s">
         <v>488</v>
       </c>
-      <c r="B231" s="2" t="s">
+      <c r="B231" t="s">
         <v>760</v>
       </c>
       <c r="C231" s="1" t="s">
@@ -8722,14 +8727,14 @@
       </c>
       <c r="G231" t="str">
         <f t="shared" si="3"/>
-        <v>K0103009802303,SASTH46@,MUHAMAD ROZAK,(XII PM),K0103009802303@gmail.com,XII PM</v>
+        <v>K0103009802303,SASTH46,MUHAMAD ROZAK,(XII PM),K0103009802303@gmail.com,XII PM</v>
       </c>
     </row>
     <row r="232" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A232" s="1" t="s">
         <v>489</v>
       </c>
-      <c r="B232" s="2" t="s">
+      <c r="B232" t="s">
         <v>760</v>
       </c>
       <c r="C232" s="1" t="s">
@@ -8746,14 +8751,14 @@
       </c>
       <c r="G232" t="str">
         <f t="shared" si="3"/>
-        <v>K0103009802312,SASTH46@,MUHAMMAD DAFFA,(XII PM),K0103009802312@gmail.com,XII PM</v>
+        <v>K0103009802312,SASTH46,MUHAMMAD DAFFA,(XII PM),K0103009802312@gmail.com,XII PM</v>
       </c>
     </row>
     <row r="233" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A233" s="1" t="s">
         <v>490</v>
       </c>
-      <c r="B233" s="2" t="s">
+      <c r="B233" t="s">
         <v>760</v>
       </c>
       <c r="C233" s="1" t="s">
@@ -8770,14 +8775,14 @@
       </c>
       <c r="G233" t="str">
         <f t="shared" si="3"/>
-        <v>K0103009802329,SASTH46@,MUHAMMAD DAFFA ANSORI,(XII PM),K0103009802329@gmail.com,XII PM</v>
+        <v>K0103009802329,SASTH46,MUHAMMAD DAFFA ANSORI,(XII PM),K0103009802329@gmail.com,XII PM</v>
       </c>
     </row>
     <row r="234" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A234" s="1" t="s">
         <v>491</v>
       </c>
-      <c r="B234" s="2" t="s">
+      <c r="B234" t="s">
         <v>760</v>
       </c>
       <c r="C234" s="1" t="s">
@@ -8794,14 +8799,14 @@
       </c>
       <c r="G234" t="str">
         <f t="shared" si="3"/>
-        <v>K0103009802338,SASTH46@,MUHAMMAD SYAH HABIANTO,(XII PM),K0103009802338@gmail.com,XII PM</v>
+        <v>K0103009802338,SASTH46,MUHAMMAD SYAH HABIANTO,(XII PM),K0103009802338@gmail.com,XII PM</v>
       </c>
     </row>
     <row r="235" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A235" s="1" t="s">
         <v>492</v>
       </c>
-      <c r="B235" s="2" t="s">
+      <c r="B235" t="s">
         <v>760</v>
       </c>
       <c r="C235" s="1" t="s">
@@ -8818,14 +8823,14 @@
       </c>
       <c r="G235" t="str">
         <f t="shared" si="3"/>
-        <v>K0103009802347,SASTH46@,NUR KHOLIS HENDAR,(XII PM),K0103009802347@gmail.com,XII PM</v>
+        <v>K0103009802347,SASTH46,NUR KHOLIS HENDAR,(XII PM),K0103009802347@gmail.com,XII PM</v>
       </c>
     </row>
     <row r="236" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A236" s="1" t="s">
         <v>493</v>
       </c>
-      <c r="B236" s="2" t="s">
+      <c r="B236" t="s">
         <v>760</v>
       </c>
       <c r="C236" s="1" t="s">
@@ -8842,14 +8847,14 @@
       </c>
       <c r="G236" t="str">
         <f t="shared" si="3"/>
-        <v>K0103009802356,SASTH46@,PENDI NUR SETIYAWAN,(XII PM),K0103009802356@gmail.com,XII PM</v>
+        <v>K0103009802356,SASTH46,PENDI NUR SETIYAWAN,(XII PM),K0103009802356@gmail.com,XII PM</v>
       </c>
     </row>
     <row r="237" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A237" s="1" t="s">
         <v>494</v>
       </c>
-      <c r="B237" s="2" t="s">
+      <c r="B237" t="s">
         <v>760</v>
       </c>
       <c r="C237" s="1" t="s">
@@ -8866,14 +8871,14 @@
       </c>
       <c r="G237" t="str">
         <f t="shared" si="3"/>
-        <v>K0103009802365,SASTH46@,RAMA ADLI ALFIAN,(XII PM),K0103009802365@gmail.com,XII PM</v>
+        <v>K0103009802365,SASTH46,RAMA ADLI ALFIAN,(XII PM),K0103009802365@gmail.com,XII PM</v>
       </c>
     </row>
     <row r="238" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A238" s="1" t="s">
         <v>495</v>
       </c>
-      <c r="B238" s="2" t="s">
+      <c r="B238" t="s">
         <v>760</v>
       </c>
       <c r="C238" s="1" t="s">
@@ -8890,14 +8895,14 @@
       </c>
       <c r="G238" t="str">
         <f t="shared" si="3"/>
-        <v>K0103009802374,SASTH46@,RIZKI ANANDA PRASETIA,(XII PM),K0103009802374@gmail.com,XII PM</v>
+        <v>K0103009802374,SASTH46,RIZKI ANANDA PRASETIA,(XII PM),K0103009802374@gmail.com,XII PM</v>
       </c>
     </row>
     <row r="239" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A239" s="1" t="s">
         <v>496</v>
       </c>
-      <c r="B239" s="2" t="s">
+      <c r="B239" t="s">
         <v>760</v>
       </c>
       <c r="C239" s="1" t="s">
@@ -8914,14 +8919,14 @@
       </c>
       <c r="G239" t="str">
         <f t="shared" si="3"/>
-        <v>K0103009802383,SASTH46@,SAFIRA ZAHRA,(XII PM),K0103009802383@gmail.com,XII PM</v>
+        <v>K0103009802383,SASTH46,SAFIRA ZAHRA,(XII PM),K0103009802383@gmail.com,XII PM</v>
       </c>
     </row>
     <row r="240" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A240" s="1" t="s">
         <v>497</v>
       </c>
-      <c r="B240" s="2" t="s">
+      <c r="B240" t="s">
         <v>760</v>
       </c>
       <c r="C240" s="1" t="s">
@@ -8938,14 +8943,14 @@
       </c>
       <c r="G240" t="str">
         <f t="shared" si="3"/>
-        <v>K0103009802392,SASTH46@,SAHRULDIN,(XII PM),K0103009802392@gmail.com,XII PM</v>
+        <v>K0103009802392,SASTH46,SAHRULDIN,(XII PM),K0103009802392@gmail.com,XII PM</v>
       </c>
     </row>
     <row r="241" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A241" s="1" t="s">
         <v>498</v>
       </c>
-      <c r="B241" s="2" t="s">
+      <c r="B241" t="s">
         <v>760</v>
       </c>
       <c r="C241" s="1" t="s">
@@ -8962,14 +8967,14 @@
       </c>
       <c r="G241" t="str">
         <f t="shared" si="3"/>
-        <v>K0103009802409,SASTH46@,SELVIA ELVINA DARAPUSPITA,(XII PM),K0103009802409@gmail.com,XII PM</v>
+        <v>K0103009802409,SASTH46,SELVIA ELVINA DARAPUSPITA,(XII PM),K0103009802409@gmail.com,XII PM</v>
       </c>
     </row>
     <row r="242" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A242" s="1" t="s">
         <v>499</v>
       </c>
-      <c r="B242" s="2" t="s">
+      <c r="B242" t="s">
         <v>760</v>
       </c>
       <c r="C242" s="1" t="s">
@@ -8986,14 +8991,14 @@
       </c>
       <c r="G242" t="str">
         <f t="shared" si="3"/>
-        <v>K0103009802418,SASTH46@,SELVY AYU DAVISTA,(XII PM),K0103009802418@gmail.com,XII PM</v>
+        <v>K0103009802418,SASTH46,SELVY AYU DAVISTA,(XII PM),K0103009802418@gmail.com,XII PM</v>
       </c>
     </row>
     <row r="243" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A243" s="1" t="s">
         <v>500</v>
       </c>
-      <c r="B243" s="2" t="s">
+      <c r="B243" t="s">
         <v>760</v>
       </c>
       <c r="C243" s="1" t="s">
@@ -9010,14 +9015,14 @@
       </c>
       <c r="G243" t="str">
         <f t="shared" si="3"/>
-        <v>K0103009802427,SASTH46@,SHANDY PUTRA IRWANSYAH,(XII PM),K0103009802427@gmail.com,XII PM</v>
+        <v>K0103009802427,SASTH46,SHANDY PUTRA IRWANSYAH,(XII PM),K0103009802427@gmail.com,XII PM</v>
       </c>
     </row>
     <row r="244" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A244" s="1" t="s">
         <v>501</v>
       </c>
-      <c r="B244" s="2" t="s">
+      <c r="B244" t="s">
         <v>760</v>
       </c>
       <c r="C244" s="1" t="s">
@@ -9034,14 +9039,14 @@
       </c>
       <c r="G244" t="str">
         <f t="shared" si="3"/>
-        <v>K0103009802436,SASTH46@,SHOHAIH AGYL SAPUTRA,(XII PM),K0103009802436@gmail.com,XII PM</v>
+        <v>K0103009802436,SASTH46,SHOHAIH AGYL SAPUTRA,(XII PM),K0103009802436@gmail.com,XII PM</v>
       </c>
     </row>
     <row r="245" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A245" s="1" t="s">
         <v>502</v>
       </c>
-      <c r="B245" s="2" t="s">
+      <c r="B245" t="s">
         <v>760</v>
       </c>
       <c r="C245" s="1" t="s">
@@ -9058,14 +9063,14 @@
       </c>
       <c r="G245" t="str">
         <f t="shared" si="3"/>
-        <v>K0103009802445,SASTH46@,SIDIK DWI MUNAHZAR,(XII PM),K0103009802445@gmail.com,XII PM</v>
+        <v>K0103009802445,SASTH46,SIDIK DWI MUNAHZAR,(XII PM),K0103009802445@gmail.com,XII PM</v>
       </c>
     </row>
     <row r="246" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A246" s="1" t="s">
         <v>503</v>
       </c>
-      <c r="B246" s="2" t="s">
+      <c r="B246" t="s">
         <v>760</v>
       </c>
       <c r="C246" s="1" t="s">
@@ -9082,14 +9087,14 @@
       </c>
       <c r="G246" t="str">
         <f t="shared" si="3"/>
-        <v>K0103009802454,SASTH46@,SYIFATUL HASANAH,(XII PM),K0103009802454@gmail.com,XII PM</v>
+        <v>K0103009802454,SASTH46,SYIFATUL HASANAH,(XII PM),K0103009802454@gmail.com,XII PM</v>
       </c>
     </row>
     <row r="247" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A247" s="1" t="s">
         <v>504</v>
       </c>
-      <c r="B247" s="2" t="s">
+      <c r="B247" t="s">
         <v>760</v>
       </c>
       <c r="C247" s="1" t="s">
@@ -9106,7 +9111,7 @@
       </c>
       <c r="G247" t="str">
         <f t="shared" si="3"/>
-        <v>K0103009802463,SASTH46@,TISYA OCTAVIA RAMADHANI,(XII PM),K0103009802463@gmail.com,XII PM</v>
+        <v>K0103009802463,SASTH46,TISYA OCTAVIA RAMADHANI,(XII PM),K0103009802463@gmail.com,XII PM</v>
       </c>
     </row>
     <row r="248" spans="1:7" x14ac:dyDescent="0.2">
@@ -14670,6 +14675,7 @@
       <c r="E1042" s="1"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="19" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>